<commit_message>
chore: update gaia_validation.xlsx & save_record tool & add level1 1 question
</commit_message>
<xml_diff>
--- a/results/GAIA/validation/gaia_validation.xlsx
+++ b/results/GAIA/validation/gaia_validation.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="25600" windowHeight="10730"/>
+    <workbookView windowWidth="28125" windowHeight="12690"/>
   </bookViews>
   <sheets>
     <sheet name="GAIA" sheetId="1" r:id="rId1"/>
@@ -17,9 +17,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="982" uniqueCount="550">
-  <si>
-    <t>THE CASTLE</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="983" uniqueCount="551">
+  <si>
+    <t>Level</t>
   </si>
   <si>
     <t>TaskID</t>
@@ -108,6 +108,9 @@
   </si>
   <si>
     <t>In Series 9, Episode 11 of Doctor Who, the Doctor is trapped inside an ever-shifting maze. What is this location called in the official script for the episode? Give the setting exactly as it appears in the first scene heading.</t>
+  </si>
+  <si>
+    <t>THE CASTLE</t>
   </si>
   <si>
     <t>1</t>
@@ -1798,8 +1801,8 @@
       <charset val="134"/>
     </font>
     <font>
+      <b/>
       <sz val="9.8"/>
-      <color rgb="FF6AAB73"/>
       <name val="Courier New"/>
       <charset val="134"/>
     </font>
@@ -2787,26 +2790,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:I166"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="I9" sqref="I9"/>
+      <selection pane="bottomLeft" activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="10" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="8.10909090909091" customWidth="1"/>
-    <col min="2" max="2" width="35.9909090909091" style="1" customWidth="1"/>
-    <col min="3" max="3" width="19.0272727272727" style="1" customWidth="1"/>
-    <col min="4" max="4" width="11.9181818181818" style="1" customWidth="1"/>
-    <col min="5" max="5" width="12.5454545454545" style="1" customWidth="1"/>
+    <col min="1" max="1" width="8.10833333333333" customWidth="1"/>
+    <col min="2" max="2" width="35.9916666666667" style="1" customWidth="1"/>
+    <col min="3" max="3" width="19.025" style="1" customWidth="1"/>
+    <col min="4" max="4" width="11.9166666666667" style="1" customWidth="1"/>
+    <col min="5" max="5" width="12.5416666666667" style="1" customWidth="1"/>
     <col min="6" max="6" width="10" style="1" customWidth="1"/>
-    <col min="7" max="7" width="7.44545454545455" style="1" customWidth="1"/>
-    <col min="8" max="8" width="6.69090909090909" style="1" customWidth="1"/>
-    <col min="9" max="9" width="9.64545454545454" style="2" customWidth="1"/>
+    <col min="7" max="7" width="7.44166666666667" style="1" customWidth="1"/>
+    <col min="8" max="8" width="6.69166666666667" style="1" customWidth="1"/>
+    <col min="9" max="9" width="9.64166666666667" style="2" customWidth="1"/>
     <col min="10" max="16378" width="10" style="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3003,10 +3006,10 @@
         <v>28</v>
       </c>
       <c r="D8" t="s">
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="E8" t="s">
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="F8" t="s">
         <v>13</v>
@@ -3015,7 +3018,7 @@
         <v>1</v>
       </c>
       <c r="I8" s="8" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" ht="14.4" customHeight="1" spans="1:9">
@@ -3023,16 +3026,16 @@
         <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C9" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D9" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E9" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F9" t="s">
         <v>13</v>
@@ -3047,16 +3050,16 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C10" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D10" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E10" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F10" t="s">
         <v>13</v>
@@ -3073,16 +3076,16 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C11" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D11" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E11" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F11" t="s">
         <v>13</v>
@@ -3099,16 +3102,16 @@
         <v>9</v>
       </c>
       <c r="B12" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C12" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D12" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E12" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F12" t="s">
         <v>13</v>
@@ -3125,16 +3128,16 @@
         <v>9</v>
       </c>
       <c r="B13" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C13" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D13" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E13" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F13" t="s">
         <v>13</v>
@@ -3151,16 +3154,16 @@
         <v>9</v>
       </c>
       <c r="B14" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C14" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D14" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E14" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F14" t="s">
         <v>13</v>
@@ -3172,21 +3175,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" ht="14" spans="1:9">
+    <row r="15" ht="13.5" spans="1:9">
       <c r="A15" t="s">
         <v>9</v>
       </c>
       <c r="B15" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C15" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F15" t="s">
         <v>13</v>
@@ -3196,21 +3199,21 @@
       </c>
       <c r="I15" s="8"/>
     </row>
-    <row r="16" ht="14" spans="1:9">
+    <row r="16" ht="13.5" spans="1:9">
       <c r="A16" t="s">
         <v>9</v>
       </c>
       <c r="B16" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C16" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D16" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E16" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="F16" t="s">
         <v>13</v>
@@ -3222,21 +3225,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" ht="14" spans="1:9">
+    <row r="17" ht="13.5" hidden="1" spans="1:9">
       <c r="A17" t="s">
         <v>9</v>
       </c>
       <c r="B17" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C17" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D17" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E17" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="F17" t="s">
         <v>13</v>
@@ -3246,21 +3249,21 @@
       </c>
       <c r="I17" s="8"/>
     </row>
-    <row r="18" ht="14" spans="1:9">
+    <row r="18" ht="13.5" hidden="1" spans="1:9">
       <c r="A18" t="s">
         <v>9</v>
       </c>
       <c r="B18" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C18" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D18" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E18" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="F18" t="s">
         <v>13</v>
@@ -3270,21 +3273,21 @@
       </c>
       <c r="I18" s="8"/>
     </row>
-    <row r="19" ht="14" spans="1:9">
+    <row r="19" ht="13.5" spans="1:9">
       <c r="A19" t="s">
         <v>9</v>
       </c>
       <c r="B19" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C19" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D19" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E19" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="F19" t="s">
         <v>13</v>
@@ -3292,23 +3295,25 @@
       <c r="G19">
         <v>1</v>
       </c>
-      <c r="I19" s="8"/>
-    </row>
-    <row r="20" ht="14" spans="1:9">
+      <c r="I19" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="20" ht="13.5" spans="1:9">
       <c r="A20" t="s">
         <v>9</v>
       </c>
       <c r="B20" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C20" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D20" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E20" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="F20" t="s">
         <v>13</v>
@@ -3318,21 +3323,21 @@
       </c>
       <c r="I20" s="8"/>
     </row>
-    <row r="21" ht="14" spans="1:9">
+    <row r="21" ht="13.5" spans="1:9">
       <c r="A21" t="s">
         <v>9</v>
       </c>
       <c r="B21" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C21" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D21" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E21" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="F21" t="s">
         <v>13</v>
@@ -3342,21 +3347,21 @@
       </c>
       <c r="I21" s="8"/>
     </row>
-    <row r="22" ht="14" spans="1:9">
+    <row r="22" ht="13.5" spans="1:9">
       <c r="A22" t="s">
         <v>9</v>
       </c>
       <c r="B22" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C22" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D22" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E22" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="F22" t="s">
         <v>13</v>
@@ -3366,21 +3371,21 @@
       </c>
       <c r="I22" s="8"/>
     </row>
-    <row r="23" ht="14" spans="1:9">
+    <row r="23" ht="13.5" hidden="1" spans="1:9">
       <c r="A23" t="s">
         <v>9</v>
       </c>
       <c r="B23" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C23" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D23" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E23" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F23" t="s">
         <v>13</v>
@@ -3390,15 +3395,15 @@
       </c>
       <c r="I23" s="8"/>
     </row>
-    <row r="24" ht="14" spans="1:9">
+    <row r="24" ht="13.5" spans="1:9">
       <c r="A24" t="s">
         <v>9</v>
       </c>
       <c r="B24" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C24" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D24" t="s">
         <v>16</v>
@@ -3414,21 +3419,21 @@
       </c>
       <c r="I24" s="8"/>
     </row>
-    <row r="25" ht="14" spans="1:9">
+    <row r="25" ht="13.5" spans="1:9">
       <c r="A25" t="s">
         <v>9</v>
       </c>
       <c r="B25" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C25" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D25" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E25" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="F25" t="s">
         <v>13</v>
@@ -3438,18 +3443,18 @@
       </c>
       <c r="I25" s="8"/>
     </row>
-    <row r="26" ht="14" spans="1:9">
+    <row r="26" ht="13.5" spans="1:9">
       <c r="A26" t="s">
         <v>9</v>
       </c>
       <c r="B26" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C26" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D26" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="E26">
         <v>4</v>
@@ -3462,21 +3467,21 @@
       </c>
       <c r="I26" s="8"/>
     </row>
-    <row r="27" ht="14" spans="1:9">
+    <row r="27" ht="13.5" spans="1:9">
       <c r="A27" t="s">
         <v>9</v>
       </c>
       <c r="B27" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C27" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D27" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E27" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="F27" t="s">
         <v>13</v>
@@ -3486,21 +3491,21 @@
       </c>
       <c r="I27" s="8"/>
     </row>
-    <row r="28" ht="14" spans="1:9">
+    <row r="28" ht="13.5" spans="1:9">
       <c r="A28" t="s">
         <v>9</v>
       </c>
       <c r="B28" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C28" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D28" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="E28" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="F28" t="s">
         <v>13</v>
@@ -3510,21 +3515,21 @@
       </c>
       <c r="I28" s="8"/>
     </row>
-    <row r="29" ht="14" spans="1:9">
+    <row r="29" ht="13.5" spans="1:9">
       <c r="A29" t="s">
         <v>9</v>
       </c>
       <c r="B29" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C29" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D29" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E29" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="F29" t="s">
         <v>13</v>
@@ -3534,21 +3539,21 @@
       </c>
       <c r="I29" s="8"/>
     </row>
-    <row r="30" ht="14" spans="1:9">
+    <row r="30" ht="13.5" spans="1:9">
       <c r="A30" t="s">
         <v>9</v>
       </c>
       <c r="B30" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C30" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D30" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="E30" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="F30" t="s">
         <v>13</v>
@@ -3558,21 +3563,21 @@
       </c>
       <c r="I30" s="8"/>
     </row>
-    <row r="31" ht="14" spans="1:9">
+    <row r="31" ht="13.5" spans="1:9">
       <c r="A31" t="s">
         <v>9</v>
       </c>
       <c r="B31" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C31" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D31" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="E31" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="F31" t="s">
         <v>13</v>
@@ -3582,21 +3587,21 @@
       </c>
       <c r="I31" s="8"/>
     </row>
-    <row r="32" ht="14" spans="1:9">
+    <row r="32" ht="13.5" spans="1:9">
       <c r="A32" t="s">
         <v>9</v>
       </c>
       <c r="B32" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C32" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D32" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="E32" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="F32" t="s">
         <v>13</v>
@@ -3606,21 +3611,21 @@
       </c>
       <c r="I32" s="8"/>
     </row>
-    <row r="33" ht="14" spans="1:9">
+    <row r="33" ht="13.5" spans="1:9">
       <c r="A33" t="s">
         <v>9</v>
       </c>
       <c r="B33" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C33" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D33" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="E33" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="F33" t="s">
         <v>13</v>
@@ -3630,21 +3635,21 @@
       </c>
       <c r="I33" s="8"/>
     </row>
-    <row r="34" ht="14" spans="1:9">
+    <row r="34" ht="13.5" spans="1:9">
       <c r="A34" t="s">
         <v>9</v>
       </c>
       <c r="B34" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C34" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D34" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="E34" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="F34" t="s">
         <v>13</v>
@@ -3654,21 +3659,21 @@
       </c>
       <c r="I34" s="8"/>
     </row>
-    <row r="35" ht="14" spans="1:9">
+    <row r="35" ht="13.5" spans="1:9">
       <c r="A35" t="s">
         <v>9</v>
       </c>
       <c r="B35" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C35" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D35" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="E35" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="F35" t="s">
         <v>13</v>
@@ -3678,21 +3683,21 @@
       </c>
       <c r="I35" s="8"/>
     </row>
-    <row r="36" ht="14" spans="1:9">
+    <row r="36" ht="13.5" spans="1:9">
       <c r="A36" t="s">
         <v>9</v>
       </c>
       <c r="B36" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C36" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D36" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="E36" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="F36" t="s">
         <v>13</v>
@@ -3702,21 +3707,21 @@
       </c>
       <c r="I36" s="8"/>
     </row>
-    <row r="37" ht="14" spans="1:9">
+    <row r="37" ht="13.5" spans="1:9">
       <c r="A37" t="s">
         <v>9</v>
       </c>
       <c r="B37" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C37" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="D37" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="E37" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="F37" t="s">
         <v>13</v>
@@ -3726,21 +3731,21 @@
       </c>
       <c r="I37" s="8"/>
     </row>
-    <row r="38" ht="14" spans="1:9">
+    <row r="38" ht="13.5" spans="1:9">
       <c r="A38" t="s">
         <v>9</v>
       </c>
       <c r="B38" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C38" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="D38" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="E38" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="F38" t="s">
         <v>13</v>
@@ -3750,21 +3755,21 @@
       </c>
       <c r="I38" s="8"/>
     </row>
-    <row r="39" ht="14" spans="1:9">
+    <row r="39" ht="13.5" spans="1:9">
       <c r="A39" t="s">
         <v>9</v>
       </c>
       <c r="B39" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C39" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="D39" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="E39" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="F39" t="s">
         <v>13</v>
@@ -3774,21 +3779,21 @@
       </c>
       <c r="I39" s="8"/>
     </row>
-    <row r="40" ht="14" spans="1:9">
+    <row r="40" ht="13.5" hidden="1" spans="1:9">
       <c r="A40" t="s">
         <v>9</v>
       </c>
       <c r="B40" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C40" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="D40" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="E40" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="F40" t="s">
         <v>13</v>
@@ -3798,21 +3803,21 @@
       </c>
       <c r="I40" s="8"/>
     </row>
-    <row r="41" ht="14" spans="1:9">
+    <row r="41" ht="13.5" spans="1:9">
       <c r="A41" t="s">
         <v>9</v>
       </c>
       <c r="B41" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C41" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D41" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="E41" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="F41" t="s">
         <v>13</v>
@@ -3822,18 +3827,18 @@
       </c>
       <c r="I41" s="8"/>
     </row>
-    <row r="42" ht="14" spans="1:9">
+    <row r="42" ht="13.5" spans="1:9">
       <c r="A42" t="s">
         <v>9</v>
       </c>
       <c r="B42" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C42" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D42" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="E42">
         <v>22</v>
@@ -3846,21 +3851,21 @@
       </c>
       <c r="I42" s="8"/>
     </row>
-    <row r="43" ht="14" spans="1:9">
+    <row r="43" ht="13.5" spans="1:9">
       <c r="A43" t="s">
         <v>9</v>
       </c>
       <c r="B43" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C43" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="D43" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="E43" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="F43" t="s">
         <v>13</v>
@@ -3870,21 +3875,21 @@
       </c>
       <c r="I43" s="8"/>
     </row>
-    <row r="44" ht="14" spans="1:9">
+    <row r="44" ht="13.5" spans="1:9">
       <c r="A44" t="s">
         <v>9</v>
       </c>
       <c r="B44" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C44" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D44" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="E44" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="F44" t="s">
         <v>13</v>
@@ -3894,21 +3899,21 @@
       </c>
       <c r="I44" s="8"/>
     </row>
-    <row r="45" ht="14" spans="1:9">
+    <row r="45" ht="13.5" spans="1:9">
       <c r="A45" t="s">
         <v>9</v>
       </c>
       <c r="B45" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C45" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D45" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E45" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F45" t="s">
         <v>13</v>
@@ -3918,21 +3923,21 @@
       </c>
       <c r="I45" s="8"/>
     </row>
-    <row r="46" ht="14" spans="1:9">
+    <row r="46" ht="13.5" spans="1:9">
       <c r="A46" t="s">
         <v>9</v>
       </c>
       <c r="B46" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C46" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D46" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="E46" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="F46" t="s">
         <v>13</v>
@@ -3942,21 +3947,21 @@
       </c>
       <c r="I46" s="8"/>
     </row>
-    <row r="47" ht="14" spans="1:9">
+    <row r="47" ht="13.5" spans="1:9">
       <c r="A47" t="s">
         <v>9</v>
       </c>
       <c r="B47" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="C47" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="D47" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="E47" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="F47" t="s">
         <v>13</v>
@@ -3966,18 +3971,18 @@
       </c>
       <c r="I47" s="8"/>
     </row>
-    <row r="48" ht="14" spans="1:9">
+    <row r="48" ht="13.5" spans="1:9">
       <c r="A48" t="s">
         <v>9</v>
       </c>
       <c r="B48" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C48" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="D48" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="E48">
         <v>90</v>
@@ -3990,21 +3995,21 @@
       </c>
       <c r="I48" s="8"/>
     </row>
-    <row r="49" ht="14" spans="1:9">
+    <row r="49" ht="13.5" spans="1:9">
       <c r="A49" t="s">
         <v>9</v>
       </c>
       <c r="B49" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C49" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="D49" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="E49" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="F49" t="s">
         <v>13</v>
@@ -4014,21 +4019,21 @@
       </c>
       <c r="I49" s="8"/>
     </row>
-    <row r="50" ht="14" spans="1:9">
+    <row r="50" ht="13.5" spans="1:9">
       <c r="A50" t="s">
         <v>9</v>
       </c>
       <c r="B50" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C50" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="D50" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="E50" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="F50" t="s">
         <v>13</v>
@@ -4038,21 +4043,21 @@
       </c>
       <c r="I50" s="8"/>
     </row>
-    <row r="51" ht="14" spans="1:9">
+    <row r="51" ht="13.5" spans="1:9">
       <c r="A51" t="s">
         <v>9</v>
       </c>
       <c r="B51" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="C51" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="D51" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="E51" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="F51" t="s">
         <v>13</v>
@@ -4062,21 +4067,21 @@
       </c>
       <c r="I51" s="8"/>
     </row>
-    <row r="52" ht="14" spans="1:9">
+    <row r="52" ht="13.5" hidden="1" spans="1:9">
       <c r="A52" t="s">
         <v>9</v>
       </c>
       <c r="B52" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C52" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="D52" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="E52" s="6" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="F52" t="s">
         <v>13</v>
@@ -4086,21 +4091,21 @@
       </c>
       <c r="I52" s="8"/>
     </row>
-    <row r="53" ht="14" spans="1:9">
+    <row r="53" ht="13.5" spans="1:9">
       <c r="A53" t="s">
         <v>9</v>
       </c>
       <c r="B53" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="C53" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="D53" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="E53" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="F53" t="s">
         <v>13</v>
@@ -4110,21 +4115,21 @@
       </c>
       <c r="I53" s="8"/>
     </row>
-    <row r="54" ht="14" spans="1:9">
+    <row r="54" ht="13.5" spans="1:9">
       <c r="A54" t="s">
         <v>9</v>
       </c>
       <c r="B54" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="C54" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="D54" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="E54" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="F54" t="s">
         <v>13</v>
@@ -4136,19 +4141,19 @@
     </row>
     <row r="55" ht="14.4" customHeight="1" spans="1:9">
       <c r="A55" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B55" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="C55" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="D55" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="E55" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="F55" t="s">
         <v>13</v>
@@ -4162,19 +4167,19 @@
     </row>
     <row r="56" ht="14.4" customHeight="1" spans="1:9">
       <c r="A56" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B56" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C56" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="D56" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="E56" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="F56" t="s">
         <v>13</v>
@@ -4188,16 +4193,16 @@
     </row>
     <row r="57" ht="14.4" customHeight="1" spans="1:9">
       <c r="A57" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B57" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C57" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="D57" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="E57">
         <v>-23.6</v>
@@ -4211,16 +4216,16 @@
     </row>
     <row r="58" ht="14.4" customHeight="1" spans="1:9">
       <c r="A58" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B58" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="C58" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="D58" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="E58">
         <v>10</v>
@@ -4234,19 +4239,19 @@
     </row>
     <row r="59" ht="14.4" customHeight="1" spans="1:9">
       <c r="A59" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B59" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="C59" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="D59" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="E59" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="F59" t="s">
         <v>13</v>
@@ -4260,19 +4265,19 @@
     </row>
     <row r="60" ht="14.4" customHeight="1" spans="1:9">
       <c r="A60" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B60" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="C60" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="D60" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="E60" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="F60" t="s">
         <v>13</v>
@@ -4286,19 +4291,19 @@
     </row>
     <row r="61" ht="14.4" customHeight="1" spans="1:9">
       <c r="A61" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B61" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="C61" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="D61" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="E61" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="F61" t="s">
         <v>13</v>
@@ -4312,19 +4317,19 @@
     </row>
     <row r="62" ht="14.4" customHeight="1" spans="1:9">
       <c r="A62" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B62" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C62" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="D62" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="E62" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="F62" t="s">
         <v>13</v>
@@ -4336,21 +4341,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" ht="14.4" customHeight="1" spans="1:9">
+    <row r="63" ht="14.4" hidden="1" customHeight="1" spans="1:9">
       <c r="A63" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B63" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="C63" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="D63" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="E63" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="F63" t="s">
         <v>13</v>
@@ -4364,19 +4369,19 @@
     </row>
     <row r="64" ht="14.4" customHeight="1" spans="1:9">
       <c r="A64" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B64" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="C64" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="D64" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="E64" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="F64" t="s">
         <v>13</v>
@@ -4388,21 +4393,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" ht="14.4" customHeight="1" spans="1:9">
+    <row r="65" ht="14.4" hidden="1" customHeight="1" spans="1:9">
       <c r="A65" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B65" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="C65" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="D65" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="E65" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="F65" t="s">
         <v>13</v>
@@ -4416,19 +4421,19 @@
     </row>
     <row r="66" ht="14.4" customHeight="1" spans="1:9">
       <c r="A66" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B66" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="C66" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="D66" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="E66" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="F66" t="s">
         <v>13</v>
@@ -4440,18 +4445,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" ht="14.4" customHeight="1" spans="1:9">
+    <row r="67" ht="14.4" hidden="1" customHeight="1" spans="1:9">
       <c r="A67" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B67" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="C67" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="D67" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="E67">
         <v>16.094</v>
@@ -4468,19 +4473,19 @@
     </row>
     <row r="68" ht="14.4" customHeight="1" spans="1:9">
       <c r="A68" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B68" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="C68" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="D68" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="E68" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="F68" t="s">
         <v>13</v>
@@ -4492,21 +4497,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" ht="14.4" customHeight="1" spans="1:9">
+    <row r="69" ht="14.4" hidden="1" customHeight="1" spans="1:9">
       <c r="A69" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B69" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="C69" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="D69" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="E69" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="F69" t="s">
         <v>13</v>
@@ -4520,19 +4525,19 @@
     </row>
     <row r="70" ht="14.4" customHeight="1" spans="1:9">
       <c r="A70" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B70" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="C70" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="D70" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="E70" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="F70" t="s">
         <v>13</v>
@@ -4544,18 +4549,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" ht="14.4" customHeight="1" spans="1:9">
+    <row r="71" ht="14.4" hidden="1" customHeight="1" spans="1:9">
       <c r="A71" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B71" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="C71" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="D71" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="E71">
         <v>9</v>
@@ -4572,19 +4577,19 @@
     </row>
     <row r="72" ht="14.4" customHeight="1" spans="1:9">
       <c r="A72" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B72" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="C72" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="D72" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="E72" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="F72" t="s">
         <v>13</v>
@@ -4596,18 +4601,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" ht="14.4" customHeight="1" spans="1:9">
+    <row r="73" ht="14.4" hidden="1" customHeight="1" spans="1:9">
       <c r="A73" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B73" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="C73" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="D73" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="E73">
         <v>52</v>
@@ -4624,13 +4629,13 @@
     </row>
     <row r="74" ht="14.4" customHeight="1" spans="1:9">
       <c r="A74" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B74" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="C74" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="D74" t="s">
         <v>12</v>
@@ -4650,19 +4655,19 @@
     </row>
     <row r="75" ht="14.4" customHeight="1" spans="1:9">
       <c r="A75" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B75" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="C75" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="D75" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="E75" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="F75" t="s">
         <v>13</v>
@@ -4676,19 +4681,19 @@
     </row>
     <row r="76" ht="14.4" customHeight="1" spans="1:9">
       <c r="A76" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B76" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="C76" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="D76" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="E76" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="F76" t="s">
         <v>13</v>
@@ -4702,13 +4707,13 @@
     </row>
     <row r="77" ht="14.4" customHeight="1" spans="1:9">
       <c r="A77" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B77" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="C77" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="D77" t="s">
         <v>16</v>
@@ -4723,21 +4728,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" ht="14.4" customHeight="1" spans="1:9">
+    <row r="78" ht="14.4" hidden="1" customHeight="1" spans="1:9">
       <c r="A78" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B78" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="C78" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="D78" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="E78" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="F78" t="s">
         <v>13</v>
@@ -4749,15 +4754,15 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="79" ht="14.4" customHeight="1" spans="1:9">
+    <row r="79" ht="14.4" hidden="1" customHeight="1" spans="1:9">
       <c r="A79" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B79" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="C79" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="D79" t="s">
         <v>16</v>
@@ -4775,18 +4780,18 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="80" ht="14.4" customHeight="1" spans="1:9">
+    <row r="80" ht="14.4" hidden="1" customHeight="1" spans="1:9">
       <c r="A80" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B80" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="C80" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="D80" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="E80" s="9">
         <v>0.711805555555556</v>
@@ -4803,19 +4808,19 @@
     </row>
     <row r="81" ht="14.4" customHeight="1" spans="1:9">
       <c r="A81" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B81" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="C81" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="D81" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="E81" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="G81">
         <v>1</v>
@@ -4826,19 +4831,19 @@
     </row>
     <row r="82" ht="14.4" customHeight="1" spans="1:9">
       <c r="A82" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B82" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="C82" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="D82" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="E82" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="G82">
         <v>1</v>
@@ -4849,19 +4854,19 @@
     </row>
     <row r="83" ht="14.4" customHeight="1" spans="1:9">
       <c r="A83" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B83" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="C83" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="D83" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="E83" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="G83">
         <v>1</v>
@@ -4872,19 +4877,19 @@
     </row>
     <row r="84" ht="14.4" customHeight="1" spans="1:9">
       <c r="A84" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B84" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="C84" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="D84" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="E84" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="F84" t="s">
         <v>13</v>
@@ -4898,19 +4903,19 @@
     </row>
     <row r="85" ht="14.4" customHeight="1" spans="1:9">
       <c r="A85" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B85" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="C85" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="D85" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="E85" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="F85" t="s">
         <v>13</v>
@@ -4924,16 +4929,16 @@
     </row>
     <row r="86" ht="14.4" customHeight="1" spans="1:9">
       <c r="A86" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B86" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="C86" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="D86" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="E86">
         <v>41</v>
@@ -4948,18 +4953,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" ht="14.4" customHeight="1" spans="1:9">
+    <row r="87" ht="14.4" hidden="1" customHeight="1" spans="1:9">
       <c r="A87" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B87" s="10" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="C87" s="10" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="D87" s="10" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="E87" s="10">
         <v>3</v>
@@ -4977,19 +4982,19 @@
     </row>
     <row r="88" ht="14.4" customHeight="1" spans="1:9">
       <c r="A88" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B88" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="C88" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="D88" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="E88" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="F88" t="s">
         <v>13</v>
@@ -5003,19 +5008,19 @@
     </row>
     <row r="89" ht="14.4" customHeight="1" spans="1:9">
       <c r="A89" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B89" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="C89" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="D89" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="E89" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="F89" t="s">
         <v>13</v>
@@ -5029,19 +5034,19 @@
     </row>
     <row r="90" ht="14.4" customHeight="1" spans="1:9">
       <c r="A90" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B90" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="C90" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="D90" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="E90" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="F90" t="s">
         <v>13</v>
@@ -5055,19 +5060,19 @@
     </row>
     <row r="91" ht="14.4" customHeight="1" spans="1:9">
       <c r="A91" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B91" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="C91" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="D91" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="E91" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="F91" t="s">
         <v>13</v>
@@ -5081,19 +5086,19 @@
     </row>
     <row r="92" ht="14.4" customHeight="1" spans="1:9">
       <c r="A92" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B92" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="C92" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="D92" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E92" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F92" t="s">
         <v>13</v>
@@ -5105,21 +5110,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="93" ht="14.4" customHeight="1" spans="1:7">
+    <row r="93" ht="14.4" hidden="1" customHeight="1" spans="1:7">
       <c r="A93" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B93" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="C93" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="D93" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="E93" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="F93" t="s">
         <v>13</v>
@@ -5128,21 +5133,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" ht="14.4" customHeight="1" spans="1:7">
+    <row r="94" ht="14.4" hidden="1" customHeight="1" spans="1:7">
       <c r="A94" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B94" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="C94" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="D94" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="E94" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="F94" t="s">
         <v>13</v>
@@ -5153,19 +5158,19 @@
     </row>
     <row r="95" ht="14.4" customHeight="1" spans="1:9">
       <c r="A95" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B95" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="C95" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="D95" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="E95" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="F95" t="s">
         <v>13</v>
@@ -5179,19 +5184,19 @@
     </row>
     <row r="96" ht="14.4" customHeight="1" spans="1:9">
       <c r="A96" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B96" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="C96" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="D96" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="E96" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="F96" t="s">
         <v>13</v>
@@ -5205,19 +5210,19 @@
     </row>
     <row r="97" ht="14.4" customHeight="1" spans="1:9">
       <c r="A97" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B97" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="C97" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="D97" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="E97" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="F97" t="s">
         <v>13</v>
@@ -5229,18 +5234,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" ht="14.4" customHeight="1" spans="1:9">
+    <row r="98" ht="14.4" hidden="1" customHeight="1" spans="1:9">
       <c r="A98" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B98" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="C98" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="D98" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="E98">
         <v>17</v>
@@ -5255,18 +5260,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" ht="14.4" customHeight="1" spans="1:7">
+    <row r="99" ht="14.4" hidden="1" customHeight="1" spans="1:7">
       <c r="A99" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B99" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="C99" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="D99" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="E99">
         <v>126</v>
@@ -5280,19 +5285,19 @@
     </row>
     <row r="100" ht="14.4" customHeight="1" spans="1:9">
       <c r="A100" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B100" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="C100" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="D100" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="E100" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="F100" t="s">
         <v>13</v>
@@ -5306,16 +5311,16 @@
     </row>
     <row r="101" ht="14.4" customHeight="1" spans="1:7">
       <c r="A101" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B101" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="C101" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="D101" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="E101">
         <v>2018</v>
@@ -5329,16 +5334,16 @@
     </row>
     <row r="102" ht="14.4" customHeight="1" spans="1:9">
       <c r="A102" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B102" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="C102" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="D102" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="E102">
         <v>0</v>
@@ -5353,21 +5358,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="103" ht="14.4" customHeight="1" spans="1:7">
+    <row r="103" ht="14.4" hidden="1" customHeight="1" spans="1:7">
       <c r="A103" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B103" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="C103" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="D103" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="E103" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="F103" t="s">
         <v>13</v>
@@ -5376,18 +5381,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" ht="14.4" customHeight="1" spans="1:7">
+    <row r="104" ht="14.4" hidden="1" customHeight="1" spans="1:7">
       <c r="A104" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B104" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="C104" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="D104" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="E104">
         <v>90</v>
@@ -5401,16 +5406,16 @@
     </row>
     <row r="105" ht="14.4" customHeight="1" spans="1:7">
       <c r="A105" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B105" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="C105" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="D105" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="E105">
         <v>13</v>
@@ -5424,16 +5429,16 @@
     </row>
     <row r="106" ht="14.4" customHeight="1" spans="1:9">
       <c r="A106" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B106" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="C106" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="D106" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="E106">
         <v>7</v>
@@ -5450,19 +5455,19 @@
     </row>
     <row r="107" ht="14.4" customHeight="1" spans="1:9">
       <c r="A107" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B107" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="C107" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="D107" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="E107" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="F107" t="s">
         <v>13</v>
@@ -5474,18 +5479,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="108" ht="14.4" customHeight="1" spans="1:9">
+    <row r="108" ht="14.4" hidden="1" customHeight="1" spans="1:9">
       <c r="A108" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B108" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="C108" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="D108" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="E108">
         <v>860000</v>
@@ -5500,21 +5505,21 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="109" ht="14.4" customHeight="1" spans="1:9">
+    <row r="109" ht="14.4" hidden="1" customHeight="1" spans="1:9">
       <c r="A109" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B109" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="C109" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="D109" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="E109" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="F109" t="s">
         <v>13</v>
@@ -5528,16 +5533,16 @@
     </row>
     <row r="110" ht="14.4" customHeight="1" spans="1:9">
       <c r="A110" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B110" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="C110" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="D110" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="E110">
         <v>563.9</v>
@@ -5554,19 +5559,19 @@
     </row>
     <row r="111" ht="14.4" customHeight="1" spans="1:7">
       <c r="A111" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B111" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="C111" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="D111" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="E111" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="F111" t="s">
         <v>13</v>
@@ -5577,19 +5582,19 @@
     </row>
     <row r="112" ht="14.4" customHeight="1" spans="1:7">
       <c r="A112" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B112" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="C112" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="D112" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="E112" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="F112" t="s">
         <v>13</v>
@@ -5600,19 +5605,19 @@
     </row>
     <row r="113" ht="14.4" customHeight="1" spans="1:7">
       <c r="A113" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B113" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="C113" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="D113" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="E113" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="F113" t="s">
         <v>13</v>
@@ -5623,19 +5628,19 @@
     </row>
     <row r="114" ht="14.4" customHeight="1" spans="1:7">
       <c r="A114" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B114" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="C114" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="D114" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="E114" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="F114" t="s">
         <v>13</v>
@@ -5646,19 +5651,19 @@
     </row>
     <row r="115" ht="14.4" customHeight="1" spans="1:7">
       <c r="A115" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B115" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="C115" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="D115" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E115" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F115" t="s">
         <v>13</v>
@@ -5667,18 +5672,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="116" ht="14.4" customHeight="1" spans="1:7">
+    <row r="116" ht="14.4" hidden="1" customHeight="1" spans="1:7">
       <c r="A116" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B116" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="C116" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="D116" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="E116">
         <v>1785</v>
@@ -5690,18 +5695,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" ht="14.4" customHeight="1" spans="1:7">
+    <row r="117" ht="14.4" hidden="1" customHeight="1" spans="1:7">
       <c r="A117" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B117" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="C117" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="D117" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="E117">
         <v>1</v>
@@ -5713,18 +5718,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" ht="14.4" customHeight="1" spans="1:7">
+    <row r="118" ht="14.4" hidden="1" customHeight="1" spans="1:7">
       <c r="A118" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B118" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="C118" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="D118" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="E118">
         <v>3</v>
@@ -5738,16 +5743,16 @@
     </row>
     <row r="119" ht="14.4" customHeight="1" spans="1:7">
       <c r="A119" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B119" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="C119" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="D119" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="E119">
         <v>60</v>
@@ -5761,19 +5766,19 @@
     </row>
     <row r="120" ht="14.4" customHeight="1" spans="1:7">
       <c r="A120" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B120" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="C120" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="D120" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="E120" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="F120" t="s">
         <v>13</v>
@@ -5784,19 +5789,19 @@
     </row>
     <row r="121" ht="14.4" customHeight="1" spans="1:7">
       <c r="A121" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B121" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="C121" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="D121" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="E121" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="F121" t="s">
         <v>13</v>
@@ -5807,19 +5812,19 @@
     </row>
     <row r="122" ht="14.4" customHeight="1" spans="1:7">
       <c r="A122" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B122" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="C122" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="D122" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="E122" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="F122" t="s">
         <v>13</v>
@@ -5830,19 +5835,19 @@
     </row>
     <row r="123" ht="14.4" customHeight="1" spans="1:7">
       <c r="A123" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B123" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="C123" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="D123" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="E123" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="F123" t="s">
         <v>13</v>
@@ -5853,16 +5858,16 @@
     </row>
     <row r="124" ht="14.4" customHeight="1" spans="1:7">
       <c r="A124" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B124" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="C124" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="D124" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="E124">
         <v>8</v>
@@ -5876,19 +5881,19 @@
     </row>
     <row r="125" ht="14.4" customHeight="1" spans="1:7">
       <c r="A125" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B125" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="C125" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="D125" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="E125" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="F125" t="s">
         <v>13</v>
@@ -5899,19 +5904,19 @@
     </row>
     <row r="126" ht="14.4" customHeight="1" spans="1:7">
       <c r="A126" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B126" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="C126" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="D126" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="E126" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="F126" t="s">
         <v>13</v>
@@ -5922,19 +5927,19 @@
     </row>
     <row r="127" ht="14.4" customHeight="1" spans="1:7">
       <c r="A127" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B127" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="C127" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="D127" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="E127" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="F127" t="s">
         <v>13</v>
@@ -5943,18 +5948,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="128" ht="14.4" customHeight="1" spans="1:9">
+    <row r="128" ht="14.4" hidden="1" customHeight="1" spans="1:9">
       <c r="A128" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B128" s="10" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="C128" s="10" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D128" s="10" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="E128" s="10">
         <v>477</v>
@@ -5970,19 +5975,19 @@
     </row>
     <row r="129" ht="14.4" customHeight="1" spans="1:7">
       <c r="A129" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B129" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="C129" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="D129" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="E129" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="F129" t="s">
         <v>13</v>
@@ -5993,19 +5998,19 @@
     </row>
     <row r="130" ht="14.4" customHeight="1" spans="1:7">
       <c r="A130" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B130" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="C130" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="D130" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="E130" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="F130" t="s">
         <v>13</v>
@@ -6016,16 +6021,16 @@
     </row>
     <row r="131" ht="14.4" customHeight="1" spans="1:7">
       <c r="A131" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B131" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="C131" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="D131" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="E131">
         <v>536</v>
@@ -6039,16 +6044,16 @@
     </row>
     <row r="132" ht="14.4" customHeight="1" spans="1:7">
       <c r="A132" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B132" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="C132" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="D132" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="E132">
         <v>1954</v>
@@ -6062,19 +6067,19 @@
     </row>
     <row r="133" ht="14.4" customHeight="1" spans="1:7">
       <c r="A133" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B133" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="C133" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="D133" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="E133" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="F133" t="s">
         <v>13</v>
@@ -6085,19 +6090,19 @@
     </row>
     <row r="134" ht="14.4" customHeight="1" spans="1:7">
       <c r="A134" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B134" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="C134" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="D134" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="E134" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="F134" t="s">
         <v>13</v>
@@ -6108,19 +6113,19 @@
     </row>
     <row r="135" ht="14.4" customHeight="1" spans="1:9">
       <c r="A135" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B135" s="10" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="C135" s="10" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="D135" s="10" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="E135" s="10" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="F135" s="10" t="s">
         <v>13</v>
@@ -6133,16 +6138,16 @@
     </row>
     <row r="136" ht="14.4" customHeight="1" spans="1:9">
       <c r="A136" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B136" s="10" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="C136" s="10" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="D136" s="10" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="E136" s="10">
         <v>116</v>
@@ -6158,19 +6163,19 @@
     </row>
     <row r="137" ht="14.4" customHeight="1" spans="1:9">
       <c r="A137" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B137" s="10" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="C137" s="10" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="D137" s="10" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="E137" s="10" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="F137" s="10" t="s">
         <v>13</v>
@@ -6183,19 +6188,19 @@
     </row>
     <row r="138" ht="14.4" customHeight="1" spans="1:7">
       <c r="A138" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B138" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="C138" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="D138" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="E138" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="F138" t="s">
         <v>13</v>
@@ -6206,62 +6211,62 @@
     </row>
     <row r="139" ht="14.4" customHeight="1" spans="1:7">
       <c r="A139" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B139" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="C139" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="D139" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="E139" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="G139">
         <v>1</v>
       </c>
     </row>
-    <row r="140" ht="14.4" customHeight="1" spans="1:7">
+    <row r="140" ht="14.4" hidden="1" customHeight="1" spans="1:7">
       <c r="A140" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B140" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="C140" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="D140" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="E140" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="F140" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="G140">
         <v>0</v>
       </c>
     </row>
-    <row r="141" ht="14.4" customHeight="1" spans="1:9">
+    <row r="141" ht="14.4" hidden="1" customHeight="1" spans="1:9">
       <c r="A141" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="B141" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="C141" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="D141" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="E141" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="F141" t="s">
         <v>13</v>
@@ -6270,25 +6275,25 @@
         <v>0</v>
       </c>
       <c r="H141" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="I141" s="8"/>
     </row>
-    <row r="142" ht="14.4" customHeight="1" spans="1:9">
+    <row r="142" ht="14.4" hidden="1" customHeight="1" spans="1:9">
       <c r="A142" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="B142" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="C142" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="D142" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="E142" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="F142" t="s">
         <v>13</v>
@@ -6297,25 +6302,25 @@
         <v>0</v>
       </c>
       <c r="H142" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="I142" s="8"/>
     </row>
     <row r="143" ht="14.4" customHeight="1" spans="1:9">
       <c r="A143" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="B143" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="C143" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="D143" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="E143" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="G143">
         <v>1</v>
@@ -6327,21 +6332,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="144" ht="14.4" customHeight="1" spans="1:9">
+    <row r="144" ht="14.4" hidden="1" customHeight="1" spans="1:9">
       <c r="A144" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="B144" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="C144" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="D144" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="E144" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="F144" t="s">
         <v>13</v>
@@ -6350,25 +6355,25 @@
         <v>0</v>
       </c>
       <c r="H144" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="I144" s="8"/>
     </row>
-    <row r="145" ht="14.4" customHeight="1" spans="1:9">
+    <row r="145" ht="14.4" hidden="1" customHeight="1" spans="1:9">
       <c r="A145" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="B145" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="C145" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="D145" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="E145" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="F145" t="s">
         <v>13</v>
@@ -6377,25 +6382,25 @@
         <v>0</v>
       </c>
       <c r="H145" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
       <c r="I145" s="8"/>
     </row>
     <row r="146" ht="14.4" customHeight="1" spans="1:9">
       <c r="A146" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="B146" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="C146" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="D146" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="E146" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="F146" t="s">
         <v>13</v>
@@ -6404,7 +6409,7 @@
         <v>1</v>
       </c>
       <c r="H146" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="I146" s="8">
         <v>1</v>
@@ -6412,19 +6417,19 @@
     </row>
     <row r="147" ht="14.4" customHeight="1" spans="1:9">
       <c r="A147" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="B147" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="C147" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="D147" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="E147" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="F147" t="s">
         <v>13</v>
@@ -6433,7 +6438,7 @@
         <v>1</v>
       </c>
       <c r="H147" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="I147" s="8">
         <v>1</v>
@@ -6441,19 +6446,19 @@
     </row>
     <row r="148" ht="14.4" customHeight="1" spans="1:9">
       <c r="A148" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="B148" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="C148" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="D148" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="E148" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="F148" t="s">
         <v>13</v>
@@ -6462,27 +6467,27 @@
         <v>1</v>
       </c>
       <c r="H148" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="I148" s="8">
         <v>1</v>
       </c>
     </row>
-    <row r="149" ht="14.4" customHeight="1" spans="1:9">
+    <row r="149" ht="14.4" hidden="1" customHeight="1" spans="1:9">
       <c r="A149" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="B149" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="C149" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="D149" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="E149" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="F149" t="s">
         <v>13</v>
@@ -6491,25 +6496,25 @@
         <v>0</v>
       </c>
       <c r="H149" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="I149" s="8"/>
     </row>
-    <row r="150" ht="14.4" customHeight="1" spans="1:9">
+    <row r="150" ht="14.4" hidden="1" customHeight="1" spans="1:9">
       <c r="A150" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="B150" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="C150" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="D150" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="E150" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="F150" t="s">
         <v>13</v>
@@ -6518,25 +6523,25 @@
         <v>0</v>
       </c>
       <c r="H150" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="I150" s="8"/>
     </row>
-    <row r="151" ht="14.4" customHeight="1" spans="1:9">
+    <row r="151" ht="14.4" hidden="1" customHeight="1" spans="1:9">
       <c r="A151" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="B151" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="C151" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
       <c r="D151" t="s">
-        <v>482</v>
+        <v>483</v>
       </c>
       <c r="E151" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="F151" t="s">
         <v>13</v>
@@ -6545,25 +6550,25 @@
         <v>0</v>
       </c>
       <c r="H151" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="I151" s="8"/>
     </row>
-    <row r="152" ht="14.4" customHeight="1" spans="1:9">
+    <row r="152" ht="14.4" hidden="1" customHeight="1" spans="1:9">
       <c r="A152" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="B152" t="s">
-        <v>485</v>
+        <v>486</v>
       </c>
       <c r="C152" t="s">
-        <v>486</v>
+        <v>487</v>
       </c>
       <c r="D152" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
       <c r="E152" t="s">
-        <v>488</v>
+        <v>489</v>
       </c>
       <c r="F152" t="s">
         <v>13</v>
@@ -6572,25 +6577,25 @@
         <v>0</v>
       </c>
       <c r="H152" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
       <c r="I152" s="8"/>
     </row>
-    <row r="153" ht="14.4" customHeight="1" spans="1:9">
+    <row r="153" ht="14.4" hidden="1" customHeight="1" spans="1:9">
       <c r="A153" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="B153" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="C153" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="D153" t="s">
-        <v>492</v>
+        <v>493</v>
       </c>
       <c r="E153" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
       <c r="F153" t="s">
         <v>13</v>
@@ -6599,25 +6604,25 @@
         <v>0</v>
       </c>
       <c r="H153" t="s">
-        <v>494</v>
+        <v>495</v>
       </c>
       <c r="I153" s="8"/>
     </row>
-    <row r="154" ht="14.4" customHeight="1" spans="1:9">
+    <row r="154" ht="14.4" hidden="1" customHeight="1" spans="1:9">
       <c r="A154" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="B154" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
       <c r="C154" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="D154" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="E154" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="F154" t="s">
         <v>13</v>
@@ -6626,25 +6631,25 @@
         <v>0</v>
       </c>
       <c r="H154" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
       <c r="I154" s="8"/>
     </row>
     <row r="155" ht="14.4" customHeight="1" spans="1:9">
       <c r="A155" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="B155" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="C155" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="D155" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="E155" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="F155" t="s">
         <v>13</v>
@@ -6653,7 +6658,7 @@
         <v>1</v>
       </c>
       <c r="H155" t="s">
-        <v>503</v>
+        <v>504</v>
       </c>
       <c r="I155" s="8">
         <v>1</v>
@@ -6661,19 +6666,19 @@
     </row>
     <row r="156" ht="14.4" customHeight="1" spans="1:9">
       <c r="A156" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="B156" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="C156" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
       <c r="D156" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
       <c r="E156" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
       <c r="F156" t="s">
         <v>13</v>
@@ -6682,27 +6687,27 @@
         <v>1</v>
       </c>
       <c r="H156" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="I156" s="8">
         <v>1</v>
       </c>
     </row>
-    <row r="157" ht="14.4" customHeight="1" spans="1:9">
+    <row r="157" ht="14.4" hidden="1" customHeight="1" spans="1:9">
       <c r="A157" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="B157" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
       <c r="C157" t="s">
-        <v>509</v>
+        <v>510</v>
       </c>
       <c r="D157" t="s">
         <v>16</v>
       </c>
       <c r="E157" t="s">
-        <v>510</v>
+        <v>511</v>
       </c>
       <c r="F157" t="s">
         <v>13</v>
@@ -6711,25 +6716,25 @@
         <v>0</v>
       </c>
       <c r="H157" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
       <c r="I157" s="8"/>
     </row>
     <row r="158" ht="14.4" customHeight="1" spans="1:9">
       <c r="A158" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="B158" t="s">
-        <v>512</v>
+        <v>513</v>
       </c>
       <c r="C158" t="s">
-        <v>513</v>
+        <v>514</v>
       </c>
       <c r="D158" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="E158" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="F158" t="s">
         <v>13</v>
@@ -6738,7 +6743,7 @@
         <v>1</v>
       </c>
       <c r="H158" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
       <c r="I158" s="8">
         <v>1</v>
@@ -6746,16 +6751,16 @@
     </row>
     <row r="159" ht="14.4" customHeight="1" spans="1:9">
       <c r="A159" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="B159" t="s">
-        <v>517</v>
+        <v>518</v>
       </c>
       <c r="C159" t="s">
-        <v>518</v>
+        <v>519</v>
       </c>
       <c r="D159" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="E159">
         <v>8</v>
@@ -6772,19 +6777,19 @@
     </row>
     <row r="160" ht="14.4" customHeight="1" spans="1:9">
       <c r="A160" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="B160" t="s">
-        <v>519</v>
+        <v>520</v>
       </c>
       <c r="C160" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
       <c r="D160" t="s">
-        <v>521</v>
+        <v>522</v>
       </c>
       <c r="E160" t="s">
-        <v>521</v>
+        <v>522</v>
       </c>
       <c r="F160" t="s">
         <v>13</v>
@@ -6793,27 +6798,27 @@
         <v>1</v>
       </c>
       <c r="H160" t="s">
-        <v>522</v>
+        <v>523</v>
       </c>
       <c r="I160" s="8">
         <v>1</v>
       </c>
     </row>
-    <row r="161" ht="14.4" customHeight="1" spans="1:9">
+    <row r="161" ht="14.4" hidden="1" customHeight="1" spans="1:9">
       <c r="A161" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="B161" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
       <c r="C161" t="s">
-        <v>524</v>
+        <v>525</v>
       </c>
       <c r="D161" t="s">
-        <v>525</v>
+        <v>526</v>
       </c>
       <c r="E161" t="s">
-        <v>526</v>
+        <v>527</v>
       </c>
       <c r="F161" t="s">
         <v>13</v>
@@ -6822,25 +6827,25 @@
         <v>0</v>
       </c>
       <c r="H161" t="s">
-        <v>527</v>
+        <v>528</v>
       </c>
       <c r="I161" s="8"/>
     </row>
-    <row r="162" ht="14.4" customHeight="1" spans="1:9">
+    <row r="162" ht="14.4" hidden="1" customHeight="1" spans="1:9">
       <c r="A162" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="B162" t="s">
-        <v>528</v>
+        <v>529</v>
       </c>
       <c r="C162" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="D162" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
       <c r="E162" t="s">
-        <v>531</v>
+        <v>532</v>
       </c>
       <c r="F162" t="s">
         <v>13</v>
@@ -6849,25 +6854,25 @@
         <v>0</v>
       </c>
       <c r="H162" t="s">
-        <v>532</v>
+        <v>533</v>
       </c>
       <c r="I162" s="8"/>
     </row>
     <row r="163" ht="14.4" customHeight="1" spans="1:9">
       <c r="A163" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="B163" t="s">
-        <v>533</v>
+        <v>534</v>
       </c>
       <c r="C163" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="D163" t="s">
-        <v>535</v>
+        <v>536</v>
       </c>
       <c r="E163" t="s">
-        <v>535</v>
+        <v>536</v>
       </c>
       <c r="F163" t="s">
         <v>13</v>
@@ -6879,21 +6884,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="164" ht="14.4" customHeight="1" spans="1:9">
+    <row r="164" ht="14.4" hidden="1" customHeight="1" spans="1:9">
       <c r="A164" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="B164" t="s">
-        <v>536</v>
+        <v>537</v>
       </c>
       <c r="C164" t="s">
-        <v>537</v>
+        <v>538</v>
       </c>
       <c r="D164" t="s">
-        <v>538</v>
+        <v>539</v>
       </c>
       <c r="E164" t="s">
-        <v>539</v>
+        <v>540</v>
       </c>
       <c r="F164" t="s">
         <v>13</v>
@@ -6902,25 +6907,25 @@
         <v>0</v>
       </c>
       <c r="H164" t="s">
-        <v>540</v>
+        <v>541</v>
       </c>
       <c r="I164" s="8"/>
     </row>
-    <row r="165" ht="14.4" customHeight="1" spans="1:9">
+    <row r="165" ht="14.4" hidden="1" customHeight="1" spans="1:9">
       <c r="A165" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="B165" t="s">
-        <v>541</v>
+        <v>542</v>
       </c>
       <c r="C165" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
       <c r="D165" t="s">
-        <v>543</v>
+        <v>544</v>
       </c>
       <c r="E165" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="F165" t="s">
         <v>13</v>
@@ -6929,25 +6934,25 @@
         <v>0</v>
       </c>
       <c r="H165" t="s">
-        <v>545</v>
+        <v>546</v>
       </c>
       <c r="I165" s="8"/>
     </row>
     <row r="166" ht="14.4" customHeight="1" spans="1:9">
       <c r="A166" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="B166" t="s">
-        <v>546</v>
+        <v>547</v>
       </c>
       <c r="C166" t="s">
-        <v>547</v>
+        <v>548</v>
       </c>
       <c r="D166" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
       <c r="E166" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
       <c r="F166" t="s">
         <v>13</v>
@@ -6956,7 +6961,7 @@
         <v>1</v>
       </c>
       <c r="H166" t="s">
-        <v>549</v>
+        <v>550</v>
       </c>
       <c r="I166" s="8">
         <v>1</v>
@@ -6964,6 +6969,11 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:XEX166">
+    <filterColumn colId="6">
+      <filters>
+        <filter val="1"/>
+      </filters>
+    </filterColumn>
     <extLst/>
   </autoFilter>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555556" footer="0.511805555555556"/>

</xml_diff>

<commit_message>
add level1 29 logfiles and level2 24 logfiles
Signed-off-by: wangalexy <wangalexy@mailto.plus>
</commit_message>
<xml_diff>
--- a/results/GAIA/validation/gaia_validation.xlsx
+++ b/results/GAIA/validation/gaia_validation.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28125" windowHeight="12690"/>
+    <workbookView windowWidth="22368" windowHeight="9564"/>
   </bookViews>
   <sheets>
     <sheet name="GAIA" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="983" uniqueCount="551">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1034" uniqueCount="551">
   <si>
     <t>Level</t>
   </si>
@@ -2790,26 +2790,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr filterMode="1"/>
+  <sheetPr/>
   <dimension ref="A1:I166"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="J6" sqref="J6"/>
+      <selection pane="bottomLeft" activeCell="J43" sqref="J43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="10" defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="1" width="8.10833333333333" customWidth="1"/>
-    <col min="2" max="2" width="35.9916666666667" style="1" customWidth="1"/>
-    <col min="3" max="3" width="19.025" style="1" customWidth="1"/>
+    <col min="1" max="1" width="8.11111111111111" customWidth="1"/>
+    <col min="2" max="2" width="35.9907407407407" style="1" customWidth="1"/>
+    <col min="3" max="3" width="19.0277777777778" style="1" customWidth="1"/>
     <col min="4" max="4" width="11.9166666666667" style="1" customWidth="1"/>
-    <col min="5" max="5" width="12.5416666666667" style="1" customWidth="1"/>
+    <col min="5" max="5" width="12.5462962962963" style="1" customWidth="1"/>
     <col min="6" max="6" width="10" style="1" customWidth="1"/>
-    <col min="7" max="7" width="7.44166666666667" style="1" customWidth="1"/>
-    <col min="8" max="8" width="6.69166666666667" style="1" customWidth="1"/>
-    <col min="9" max="9" width="9.64166666666667" style="2" customWidth="1"/>
+    <col min="7" max="7" width="7.44444444444444" style="1" customWidth="1"/>
+    <col min="8" max="8" width="6.69444444444444" style="1" customWidth="1"/>
+    <col min="9" max="9" width="9.63888888888889" style="2" customWidth="1"/>
     <col min="10" max="16378" width="10" style="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3043,7 +3043,9 @@
       <c r="G9">
         <v>1</v>
       </c>
-      <c r="I9" s="8"/>
+      <c r="I9" s="8" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="10" ht="14.4" customHeight="1" spans="1:9">
       <c r="A10" t="s">
@@ -3175,7 +3177,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" ht="13.5" spans="1:9">
+    <row r="15" ht="14.4" spans="1:9">
       <c r="A15" t="s">
         <v>9</v>
       </c>
@@ -3197,9 +3199,11 @@
       <c r="G15">
         <v>1</v>
       </c>
-      <c r="I15" s="8"/>
-    </row>
-    <row r="16" ht="13.5" spans="1:9">
+      <c r="I15" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" ht="14.4" spans="1:9">
       <c r="A16" t="s">
         <v>9</v>
       </c>
@@ -3225,7 +3229,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" ht="13.5" hidden="1" spans="1:9">
+    <row r="17" ht="14.4" spans="1:9">
       <c r="A17" t="s">
         <v>9</v>
       </c>
@@ -3249,7 +3253,7 @@
       </c>
       <c r="I17" s="8"/>
     </row>
-    <row r="18" ht="13.5" hidden="1" spans="1:9">
+    <row r="18" ht="14.4" spans="1:9">
       <c r="A18" t="s">
         <v>9</v>
       </c>
@@ -3273,7 +3277,7 @@
       </c>
       <c r="I18" s="8"/>
     </row>
-    <row r="19" ht="13.5" spans="1:9">
+    <row r="19" ht="14.4" spans="1:9">
       <c r="A19" t="s">
         <v>9</v>
       </c>
@@ -3299,7 +3303,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="20" ht="13.5" spans="1:9">
+    <row r="20" ht="14.4" spans="1:9">
       <c r="A20" t="s">
         <v>9</v>
       </c>
@@ -3321,9 +3325,11 @@
       <c r="G20">
         <v>1</v>
       </c>
-      <c r="I20" s="8"/>
-    </row>
-    <row r="21" ht="13.5" spans="1:9">
+      <c r="I20" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21" ht="14.4" spans="1:9">
       <c r="A21" t="s">
         <v>9</v>
       </c>
@@ -3345,9 +3351,11 @@
       <c r="G21">
         <v>1</v>
       </c>
-      <c r="I21" s="8"/>
-    </row>
-    <row r="22" ht="13.5" spans="1:9">
+      <c r="I21" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="22" ht="14.4" spans="1:9">
       <c r="A22" t="s">
         <v>9</v>
       </c>
@@ -3369,9 +3377,11 @@
       <c r="G22">
         <v>1</v>
       </c>
-      <c r="I22" s="8"/>
-    </row>
-    <row r="23" ht="13.5" hidden="1" spans="1:9">
+      <c r="I22" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="23" ht="14.4" spans="1:9">
       <c r="A23" t="s">
         <v>9</v>
       </c>
@@ -3395,7 +3405,7 @@
       </c>
       <c r="I23" s="8"/>
     </row>
-    <row r="24" ht="13.5" spans="1:9">
+    <row r="24" ht="14.4" spans="1:9">
       <c r="A24" t="s">
         <v>9</v>
       </c>
@@ -3417,9 +3427,11 @@
       <c r="G24">
         <v>1</v>
       </c>
-      <c r="I24" s="8"/>
-    </row>
-    <row r="25" ht="13.5" spans="1:9">
+      <c r="I24" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="25" ht="14.4" spans="1:9">
       <c r="A25" t="s">
         <v>9</v>
       </c>
@@ -3441,9 +3453,11 @@
       <c r="G25">
         <v>1</v>
       </c>
-      <c r="I25" s="8"/>
-    </row>
-    <row r="26" ht="13.5" spans="1:9">
+      <c r="I25" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="26" ht="14.4" spans="1:9">
       <c r="A26" t="s">
         <v>9</v>
       </c>
@@ -3465,9 +3479,11 @@
       <c r="G26">
         <v>1</v>
       </c>
-      <c r="I26" s="8"/>
-    </row>
-    <row r="27" ht="13.5" spans="1:9">
+      <c r="I26" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="27" ht="14.4" spans="1:9">
       <c r="A27" t="s">
         <v>9</v>
       </c>
@@ -3489,9 +3505,11 @@
       <c r="G27">
         <v>1</v>
       </c>
-      <c r="I27" s="8"/>
-    </row>
-    <row r="28" ht="13.5" spans="1:9">
+      <c r="I27" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="28" ht="14.4" spans="1:9">
       <c r="A28" t="s">
         <v>9</v>
       </c>
@@ -3513,9 +3531,11 @@
       <c r="G28">
         <v>1</v>
       </c>
-      <c r="I28" s="8"/>
-    </row>
-    <row r="29" ht="13.5" spans="1:9">
+      <c r="I28" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="29" ht="14.4" spans="1:9">
       <c r="A29" t="s">
         <v>9</v>
       </c>
@@ -3537,9 +3557,11 @@
       <c r="G29">
         <v>1</v>
       </c>
-      <c r="I29" s="8"/>
-    </row>
-    <row r="30" ht="13.5" spans="1:9">
+      <c r="I29" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="30" ht="14.4" spans="1:9">
       <c r="A30" t="s">
         <v>9</v>
       </c>
@@ -3561,9 +3583,11 @@
       <c r="G30">
         <v>1</v>
       </c>
-      <c r="I30" s="8"/>
-    </row>
-    <row r="31" ht="13.5" spans="1:9">
+      <c r="I30" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="31" ht="14.4" spans="1:9">
       <c r="A31" t="s">
         <v>9</v>
       </c>
@@ -3585,9 +3609,11 @@
       <c r="G31">
         <v>1</v>
       </c>
-      <c r="I31" s="8"/>
-    </row>
-    <row r="32" ht="13.5" spans="1:9">
+      <c r="I31" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" ht="14.4" spans="1:9">
       <c r="A32" t="s">
         <v>9</v>
       </c>
@@ -3609,9 +3635,11 @@
       <c r="G32">
         <v>1</v>
       </c>
-      <c r="I32" s="8"/>
-    </row>
-    <row r="33" ht="13.5" spans="1:9">
+      <c r="I32" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="33" ht="14.4" spans="1:9">
       <c r="A33" t="s">
         <v>9</v>
       </c>
@@ -3633,9 +3661,11 @@
       <c r="G33">
         <v>1</v>
       </c>
-      <c r="I33" s="8"/>
-    </row>
-    <row r="34" ht="13.5" spans="1:9">
+      <c r="I33" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="34" ht="14.4" spans="1:9">
       <c r="A34" t="s">
         <v>9</v>
       </c>
@@ -3657,9 +3687,11 @@
       <c r="G34">
         <v>1</v>
       </c>
-      <c r="I34" s="8"/>
-    </row>
-    <row r="35" ht="13.5" spans="1:9">
+      <c r="I34" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="35" ht="14.4" spans="1:9">
       <c r="A35" t="s">
         <v>9</v>
       </c>
@@ -3681,9 +3713,11 @@
       <c r="G35">
         <v>1</v>
       </c>
-      <c r="I35" s="8"/>
-    </row>
-    <row r="36" ht="13.5" spans="1:9">
+      <c r="I35" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="36" ht="14.4" spans="1:9">
       <c r="A36" t="s">
         <v>9</v>
       </c>
@@ -3705,9 +3739,11 @@
       <c r="G36">
         <v>1</v>
       </c>
-      <c r="I36" s="8"/>
-    </row>
-    <row r="37" ht="13.5" spans="1:9">
+      <c r="I36" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="37" ht="14.4" spans="1:9">
       <c r="A37" t="s">
         <v>9</v>
       </c>
@@ -3729,9 +3765,11 @@
       <c r="G37">
         <v>1</v>
       </c>
-      <c r="I37" s="8"/>
-    </row>
-    <row r="38" ht="13.5" spans="1:9">
+      <c r="I37" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="38" ht="14.4" spans="1:9">
       <c r="A38" t="s">
         <v>9</v>
       </c>
@@ -3753,9 +3791,11 @@
       <c r="G38">
         <v>1</v>
       </c>
-      <c r="I38" s="8"/>
-    </row>
-    <row r="39" ht="13.5" spans="1:9">
+      <c r="I38" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="39" ht="14.4" spans="1:9">
       <c r="A39" t="s">
         <v>9</v>
       </c>
@@ -3779,7 +3819,7 @@
       </c>
       <c r="I39" s="8"/>
     </row>
-    <row r="40" ht="13.5" hidden="1" spans="1:9">
+    <row r="40" ht="14.4" spans="1:9">
       <c r="A40" t="s">
         <v>9</v>
       </c>
@@ -3803,7 +3843,7 @@
       </c>
       <c r="I40" s="8"/>
     </row>
-    <row r="41" ht="13.5" spans="1:9">
+    <row r="41" ht="14.4" spans="1:9">
       <c r="A41" t="s">
         <v>9</v>
       </c>
@@ -3827,7 +3867,7 @@
       </c>
       <c r="I41" s="8"/>
     </row>
-    <row r="42" ht="13.5" spans="1:9">
+    <row r="42" ht="14.4" spans="1:9">
       <c r="A42" t="s">
         <v>9</v>
       </c>
@@ -3849,9 +3889,11 @@
       <c r="G42">
         <v>1</v>
       </c>
-      <c r="I42" s="8"/>
-    </row>
-    <row r="43" ht="13.5" spans="1:9">
+      <c r="I42" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="43" ht="14.4" spans="1:9">
       <c r="A43" t="s">
         <v>9</v>
       </c>
@@ -3873,9 +3915,11 @@
       <c r="G43">
         <v>1</v>
       </c>
-      <c r="I43" s="8"/>
-    </row>
-    <row r="44" ht="13.5" spans="1:9">
+      <c r="I43" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="44" ht="14.4" spans="1:9">
       <c r="A44" t="s">
         <v>9</v>
       </c>
@@ -3897,9 +3941,11 @@
       <c r="G44">
         <v>1</v>
       </c>
-      <c r="I44" s="8"/>
-    </row>
-    <row r="45" ht="13.5" spans="1:9">
+      <c r="I44" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="45" ht="14.4" spans="1:9">
       <c r="A45" t="s">
         <v>9</v>
       </c>
@@ -3921,9 +3967,11 @@
       <c r="G45">
         <v>1</v>
       </c>
-      <c r="I45" s="8"/>
-    </row>
-    <row r="46" ht="13.5" spans="1:9">
+      <c r="I45" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="46" ht="14.4" spans="1:9">
       <c r="A46" t="s">
         <v>9</v>
       </c>
@@ -3947,7 +3995,7 @@
       </c>
       <c r="I46" s="8"/>
     </row>
-    <row r="47" ht="13.5" spans="1:9">
+    <row r="47" ht="14.4" spans="1:9">
       <c r="A47" t="s">
         <v>9</v>
       </c>
@@ -3969,9 +4017,11 @@
       <c r="G47">
         <v>1</v>
       </c>
-      <c r="I47" s="8"/>
-    </row>
-    <row r="48" ht="13.5" spans="1:9">
+      <c r="I47" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="48" ht="14.4" spans="1:9">
       <c r="A48" t="s">
         <v>9</v>
       </c>
@@ -3993,9 +4043,11 @@
       <c r="G48">
         <v>1</v>
       </c>
-      <c r="I48" s="8"/>
-    </row>
-    <row r="49" ht="13.5" spans="1:9">
+      <c r="I48" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="49" ht="14.4" spans="1:9">
       <c r="A49" t="s">
         <v>9</v>
       </c>
@@ -4017,9 +4069,11 @@
       <c r="G49">
         <v>1</v>
       </c>
-      <c r="I49" s="8"/>
-    </row>
-    <row r="50" ht="13.5" spans="1:9">
+      <c r="I49" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="50" ht="14.4" spans="1:9">
       <c r="A50" t="s">
         <v>9</v>
       </c>
@@ -4041,9 +4095,11 @@
       <c r="G50">
         <v>1</v>
       </c>
-      <c r="I50" s="8"/>
-    </row>
-    <row r="51" ht="13.5" spans="1:9">
+      <c r="I50" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="51" ht="14.4" spans="1:9">
       <c r="A51" t="s">
         <v>9</v>
       </c>
@@ -4067,7 +4123,7 @@
       </c>
       <c r="I51" s="8"/>
     </row>
-    <row r="52" ht="13.5" hidden="1" spans="1:9">
+    <row r="52" ht="14.4" spans="1:9">
       <c r="A52" t="s">
         <v>9</v>
       </c>
@@ -4091,7 +4147,7 @@
       </c>
       <c r="I52" s="8"/>
     </row>
-    <row r="53" ht="13.5" spans="1:9">
+    <row r="53" ht="14.4" spans="1:9">
       <c r="A53" t="s">
         <v>9</v>
       </c>
@@ -4113,9 +4169,11 @@
       <c r="G53">
         <v>1</v>
       </c>
-      <c r="I53" s="8"/>
-    </row>
-    <row r="54" ht="13.5" spans="1:9">
+      <c r="I53" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="54" ht="14.4" spans="1:9">
       <c r="A54" t="s">
         <v>9</v>
       </c>
@@ -4137,7 +4195,9 @@
       <c r="G54">
         <v>1</v>
       </c>
-      <c r="I54" s="8"/>
+      <c r="I54" s="8" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="55" ht="14.4" customHeight="1" spans="1:9">
       <c r="A55" t="s">
@@ -4341,7 +4401,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" ht="14.4" hidden="1" customHeight="1" spans="1:9">
+    <row r="63" ht="14.4" customHeight="1" spans="1:9">
       <c r="A63" t="s">
         <v>175</v>
       </c>
@@ -4393,7 +4453,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" ht="14.4" hidden="1" customHeight="1" spans="1:9">
+    <row r="65" ht="14.4" customHeight="1" spans="1:9">
       <c r="A65" t="s">
         <v>175</v>
       </c>
@@ -4445,7 +4505,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" ht="14.4" hidden="1" customHeight="1" spans="1:9">
+    <row r="67" ht="14.4" customHeight="1" spans="1:9">
       <c r="A67" t="s">
         <v>175</v>
       </c>
@@ -4497,7 +4557,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" ht="14.4" hidden="1" customHeight="1" spans="1:9">
+    <row r="69" ht="14.4" customHeight="1" spans="1:9">
       <c r="A69" t="s">
         <v>175</v>
       </c>
@@ -4549,7 +4609,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" ht="14.4" hidden="1" customHeight="1" spans="1:9">
+    <row r="71" ht="14.4" customHeight="1" spans="1:9">
       <c r="A71" t="s">
         <v>175</v>
       </c>
@@ -4601,7 +4661,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" ht="14.4" hidden="1" customHeight="1" spans="1:9">
+    <row r="73" ht="14.4" customHeight="1" spans="1:9">
       <c r="A73" t="s">
         <v>175</v>
       </c>
@@ -4728,7 +4788,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" ht="14.4" hidden="1" customHeight="1" spans="1:9">
+    <row r="78" ht="14.4" customHeight="1" spans="1:9">
       <c r="A78" t="s">
         <v>175</v>
       </c>
@@ -4754,7 +4814,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="79" ht="14.4" hidden="1" customHeight="1" spans="1:9">
+    <row r="79" ht="14.4" customHeight="1" spans="1:9">
       <c r="A79" t="s">
         <v>175</v>
       </c>
@@ -4780,7 +4840,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="80" ht="14.4" hidden="1" customHeight="1" spans="1:9">
+    <row r="80" ht="14.4" customHeight="1" spans="1:9">
       <c r="A80" t="s">
         <v>175</v>
       </c>
@@ -4953,7 +5013,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" ht="14.4" hidden="1" customHeight="1" spans="1:9">
+    <row r="87" ht="14.4" customHeight="1" spans="1:9">
       <c r="A87" t="s">
         <v>175</v>
       </c>
@@ -5110,7 +5170,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="93" ht="14.4" hidden="1" customHeight="1" spans="1:7">
+    <row r="93" ht="14.4" customHeight="1" spans="1:7">
       <c r="A93" t="s">
         <v>175</v>
       </c>
@@ -5133,7 +5193,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" ht="14.4" hidden="1" customHeight="1" spans="1:7">
+    <row r="94" ht="14.4" customHeight="1" spans="1:7">
       <c r="A94" t="s">
         <v>175</v>
       </c>
@@ -5234,7 +5294,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" ht="14.4" hidden="1" customHeight="1" spans="1:9">
+    <row r="98" ht="14.4" customHeight="1" spans="1:9">
       <c r="A98" t="s">
         <v>175</v>
       </c>
@@ -5260,7 +5320,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" ht="14.4" hidden="1" customHeight="1" spans="1:7">
+    <row r="99" ht="14.4" customHeight="1" spans="1:7">
       <c r="A99" t="s">
         <v>175</v>
       </c>
@@ -5358,7 +5418,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="103" ht="14.4" hidden="1" customHeight="1" spans="1:7">
+    <row r="103" ht="14.4" customHeight="1" spans="1:7">
       <c r="A103" t="s">
         <v>175</v>
       </c>
@@ -5381,7 +5441,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" ht="14.4" hidden="1" customHeight="1" spans="1:7">
+    <row r="104" ht="14.4" customHeight="1" spans="1:7">
       <c r="A104" t="s">
         <v>175</v>
       </c>
@@ -5479,7 +5539,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="108" ht="14.4" hidden="1" customHeight="1" spans="1:9">
+    <row r="108" ht="14.4" customHeight="1" spans="1:9">
       <c r="A108" t="s">
         <v>175</v>
       </c>
@@ -5505,7 +5565,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="109" ht="14.4" hidden="1" customHeight="1" spans="1:9">
+    <row r="109" ht="14.4" customHeight="1" spans="1:9">
       <c r="A109" t="s">
         <v>175</v>
       </c>
@@ -5557,7 +5617,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="111" ht="14.4" customHeight="1" spans="1:7">
+    <row r="111" ht="14.4" customHeight="1" spans="1:9">
       <c r="A111" t="s">
         <v>175</v>
       </c>
@@ -5579,8 +5639,11 @@
       <c r="G111">
         <v>1</v>
       </c>
-    </row>
-    <row r="112" ht="14.4" customHeight="1" spans="1:7">
+      <c r="I111" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="112" ht="14.4" customHeight="1" spans="1:9">
       <c r="A112" t="s">
         <v>175</v>
       </c>
@@ -5602,8 +5665,11 @@
       <c r="G112">
         <v>1</v>
       </c>
-    </row>
-    <row r="113" ht="14.4" customHeight="1" spans="1:7">
+      <c r="I112" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="113" ht="14.4" customHeight="1" spans="1:9">
       <c r="A113" t="s">
         <v>175</v>
       </c>
@@ -5625,8 +5691,11 @@
       <c r="G113">
         <v>1</v>
       </c>
-    </row>
-    <row r="114" ht="14.4" customHeight="1" spans="1:7">
+      <c r="I113" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="114" ht="14.4" customHeight="1" spans="1:9">
       <c r="A114" t="s">
         <v>175</v>
       </c>
@@ -5648,8 +5717,11 @@
       <c r="G114">
         <v>1</v>
       </c>
-    </row>
-    <row r="115" ht="14.4" customHeight="1" spans="1:7">
+      <c r="I114" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="115" ht="14.4" customHeight="1" spans="1:9">
       <c r="A115" t="s">
         <v>175</v>
       </c>
@@ -5671,8 +5743,11 @@
       <c r="G115">
         <v>1</v>
       </c>
-    </row>
-    <row r="116" ht="14.4" hidden="1" customHeight="1" spans="1:7">
+      <c r="I115" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="116" ht="14.4" customHeight="1" spans="1:7">
       <c r="A116" t="s">
         <v>175</v>
       </c>
@@ -5695,7 +5770,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" ht="14.4" hidden="1" customHeight="1" spans="1:7">
+    <row r="117" ht="14.4" customHeight="1" spans="1:7">
       <c r="A117" t="s">
         <v>175</v>
       </c>
@@ -5718,7 +5793,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" ht="14.4" hidden="1" customHeight="1" spans="1:7">
+    <row r="118" ht="14.4" customHeight="1" spans="1:7">
       <c r="A118" t="s">
         <v>175</v>
       </c>
@@ -5741,7 +5816,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" ht="14.4" customHeight="1" spans="1:7">
+    <row r="119" ht="14.4" customHeight="1" spans="1:9">
       <c r="A119" t="s">
         <v>175</v>
       </c>
@@ -5763,8 +5838,11 @@
       <c r="G119">
         <v>1</v>
       </c>
-    </row>
-    <row r="120" ht="14.4" customHeight="1" spans="1:7">
+      <c r="I119" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="120" ht="14.4" customHeight="1" spans="1:9">
       <c r="A120" t="s">
         <v>175</v>
       </c>
@@ -5786,8 +5864,11 @@
       <c r="G120">
         <v>1</v>
       </c>
-    </row>
-    <row r="121" ht="14.4" customHeight="1" spans="1:7">
+      <c r="I120" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="121" ht="14.4" customHeight="1" spans="1:9">
       <c r="A121" t="s">
         <v>175</v>
       </c>
@@ -5809,8 +5890,11 @@
       <c r="G121">
         <v>1</v>
       </c>
-    </row>
-    <row r="122" ht="14.4" customHeight="1" spans="1:7">
+      <c r="I121" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="122" ht="14.4" customHeight="1" spans="1:9">
       <c r="A122" t="s">
         <v>175</v>
       </c>
@@ -5832,8 +5916,11 @@
       <c r="G122">
         <v>1</v>
       </c>
-    </row>
-    <row r="123" ht="14.4" customHeight="1" spans="1:7">
+      <c r="I122" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="123" ht="14.4" customHeight="1" spans="1:9">
       <c r="A123" t="s">
         <v>175</v>
       </c>
@@ -5855,8 +5942,11 @@
       <c r="G123">
         <v>1</v>
       </c>
-    </row>
-    <row r="124" ht="14.4" customHeight="1" spans="1:7">
+      <c r="I123" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="124" ht="14.4" customHeight="1" spans="1:9">
       <c r="A124" t="s">
         <v>175</v>
       </c>
@@ -5878,8 +5968,11 @@
       <c r="G124">
         <v>1</v>
       </c>
-    </row>
-    <row r="125" ht="14.4" customHeight="1" spans="1:7">
+      <c r="I124" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="125" ht="14.4" customHeight="1" spans="1:9">
       <c r="A125" t="s">
         <v>175</v>
       </c>
@@ -5901,8 +5994,11 @@
       <c r="G125">
         <v>1</v>
       </c>
-    </row>
-    <row r="126" ht="14.4" customHeight="1" spans="1:7">
+      <c r="I125" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="126" ht="14.4" customHeight="1" spans="1:9">
       <c r="A126" t="s">
         <v>175</v>
       </c>
@@ -5924,6 +6020,9 @@
       <c r="G126">
         <v>1</v>
       </c>
+      <c r="I126" s="2" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="127" ht="14.4" customHeight="1" spans="1:7">
       <c r="A127" t="s">
@@ -5948,7 +6047,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="128" ht="14.4" hidden="1" customHeight="1" spans="1:9">
+    <row r="128" ht="14.4" customHeight="1" spans="1:9">
       <c r="A128" t="s">
         <v>175</v>
       </c>
@@ -5973,7 +6072,7 @@
       <c r="H128" s="10"/>
       <c r="I128" s="10"/>
     </row>
-    <row r="129" ht="14.4" customHeight="1" spans="1:7">
+    <row r="129" ht="14.4" customHeight="1" spans="1:9">
       <c r="A129" t="s">
         <v>175</v>
       </c>
@@ -5995,8 +6094,11 @@
       <c r="G129">
         <v>1</v>
       </c>
-    </row>
-    <row r="130" ht="14.4" customHeight="1" spans="1:7">
+      <c r="I129" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="130" ht="14.4" customHeight="1" spans="1:9">
       <c r="A130" t="s">
         <v>175</v>
       </c>
@@ -6018,8 +6120,11 @@
       <c r="G130">
         <v>1</v>
       </c>
-    </row>
-    <row r="131" ht="14.4" customHeight="1" spans="1:7">
+      <c r="I130" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="131" ht="14.4" customHeight="1" spans="1:9">
       <c r="A131" t="s">
         <v>175</v>
       </c>
@@ -6041,8 +6146,11 @@
       <c r="G131">
         <v>1</v>
       </c>
-    </row>
-    <row r="132" ht="14.4" customHeight="1" spans="1:7">
+      <c r="I131" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="132" ht="14.4" customHeight="1" spans="1:9">
       <c r="A132" t="s">
         <v>175</v>
       </c>
@@ -6064,8 +6172,11 @@
       <c r="G132">
         <v>1</v>
       </c>
-    </row>
-    <row r="133" ht="14.4" customHeight="1" spans="1:7">
+      <c r="I132" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="133" ht="14.4" customHeight="1" spans="1:9">
       <c r="A133" t="s">
         <v>175</v>
       </c>
@@ -6087,8 +6198,11 @@
       <c r="G133">
         <v>1</v>
       </c>
-    </row>
-    <row r="134" ht="14.4" customHeight="1" spans="1:7">
+      <c r="I133" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="134" ht="14.4" customHeight="1" spans="1:9">
       <c r="A134" t="s">
         <v>175</v>
       </c>
@@ -6110,6 +6224,9 @@
       <c r="G134">
         <v>1</v>
       </c>
+      <c r="I134" s="2" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="135" ht="14.4" customHeight="1" spans="1:9">
       <c r="A135" t="s">
@@ -6134,7 +6251,9 @@
         <v>1</v>
       </c>
       <c r="H135" s="10"/>
-      <c r="I135" s="10"/>
+      <c r="I135" s="10">
+        <v>1</v>
+      </c>
     </row>
     <row r="136" ht="14.4" customHeight="1" spans="1:9">
       <c r="A136" t="s">
@@ -6159,7 +6278,9 @@
         <v>1</v>
       </c>
       <c r="H136" s="10"/>
-      <c r="I136" s="10"/>
+      <c r="I136" s="10">
+        <v>1</v>
+      </c>
     </row>
     <row r="137" ht="14.4" customHeight="1" spans="1:9">
       <c r="A137" t="s">
@@ -6184,9 +6305,11 @@
         <v>1</v>
       </c>
       <c r="H137" s="10"/>
-      <c r="I137" s="10"/>
-    </row>
-    <row r="138" ht="14.4" customHeight="1" spans="1:7">
+      <c r="I137" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="138" ht="14.4" customHeight="1" spans="1:9">
       <c r="A138" t="s">
         <v>175</v>
       </c>
@@ -6208,8 +6331,11 @@
       <c r="G138">
         <v>1</v>
       </c>
-    </row>
-    <row r="139" ht="14.4" customHeight="1" spans="1:7">
+      <c r="I138" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="139" ht="14.4" customHeight="1" spans="1:9">
       <c r="A139" t="s">
         <v>175</v>
       </c>
@@ -6228,8 +6354,11 @@
       <c r="G139">
         <v>1</v>
       </c>
-    </row>
-    <row r="140" ht="14.4" hidden="1" customHeight="1" spans="1:7">
+      <c r="I139" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="140" ht="14.4" customHeight="1" spans="1:7">
       <c r="A140" t="s">
         <v>175</v>
       </c>
@@ -6252,7 +6381,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="141" ht="14.4" hidden="1" customHeight="1" spans="1:9">
+    <row r="141" ht="14.4" customHeight="1" spans="1:9">
       <c r="A141" t="s">
         <v>437</v>
       </c>
@@ -6279,7 +6408,7 @@
       </c>
       <c r="I141" s="8"/>
     </row>
-    <row r="142" ht="14.4" hidden="1" customHeight="1" spans="1:9">
+    <row r="142" ht="14.4" customHeight="1" spans="1:9">
       <c r="A142" t="s">
         <v>437</v>
       </c>
@@ -6332,7 +6461,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="144" ht="14.4" hidden="1" customHeight="1" spans="1:9">
+    <row r="144" ht="14.4" customHeight="1" spans="1:9">
       <c r="A144" t="s">
         <v>437</v>
       </c>
@@ -6359,7 +6488,7 @@
       </c>
       <c r="I144" s="8"/>
     </row>
-    <row r="145" ht="14.4" hidden="1" customHeight="1" spans="1:9">
+    <row r="145" ht="14.4" customHeight="1" spans="1:9">
       <c r="A145" t="s">
         <v>437</v>
       </c>
@@ -6473,7 +6602,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="149" ht="14.4" hidden="1" customHeight="1" spans="1:9">
+    <row r="149" ht="14.4" customHeight="1" spans="1:9">
       <c r="A149" t="s">
         <v>437</v>
       </c>
@@ -6500,7 +6629,7 @@
       </c>
       <c r="I149" s="8"/>
     </row>
-    <row r="150" ht="14.4" hidden="1" customHeight="1" spans="1:9">
+    <row r="150" ht="14.4" customHeight="1" spans="1:9">
       <c r="A150" t="s">
         <v>437</v>
       </c>
@@ -6527,7 +6656,7 @@
       </c>
       <c r="I150" s="8"/>
     </row>
-    <row r="151" ht="14.4" hidden="1" customHeight="1" spans="1:9">
+    <row r="151" ht="14.4" customHeight="1" spans="1:9">
       <c r="A151" t="s">
         <v>437</v>
       </c>
@@ -6554,7 +6683,7 @@
       </c>
       <c r="I151" s="8"/>
     </row>
-    <row r="152" ht="14.4" hidden="1" customHeight="1" spans="1:9">
+    <row r="152" ht="14.4" customHeight="1" spans="1:9">
       <c r="A152" t="s">
         <v>437</v>
       </c>
@@ -6581,7 +6710,7 @@
       </c>
       <c r="I152" s="8"/>
     </row>
-    <row r="153" ht="14.4" hidden="1" customHeight="1" spans="1:9">
+    <row r="153" ht="14.4" customHeight="1" spans="1:9">
       <c r="A153" t="s">
         <v>437</v>
       </c>
@@ -6608,7 +6737,7 @@
       </c>
       <c r="I153" s="8"/>
     </row>
-    <row r="154" ht="14.4" hidden="1" customHeight="1" spans="1:9">
+    <row r="154" ht="14.4" customHeight="1" spans="1:9">
       <c r="A154" t="s">
         <v>437</v>
       </c>
@@ -6693,7 +6822,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="157" ht="14.4" hidden="1" customHeight="1" spans="1:9">
+    <row r="157" ht="14.4" customHeight="1" spans="1:9">
       <c r="A157" t="s">
         <v>437</v>
       </c>
@@ -6804,7 +6933,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="161" ht="14.4" hidden="1" customHeight="1" spans="1:9">
+    <row r="161" ht="14.4" customHeight="1" spans="1:9">
       <c r="A161" t="s">
         <v>437</v>
       </c>
@@ -6831,7 +6960,7 @@
       </c>
       <c r="I161" s="8"/>
     </row>
-    <row r="162" ht="14.4" hidden="1" customHeight="1" spans="1:9">
+    <row r="162" ht="14.4" customHeight="1" spans="1:9">
       <c r="A162" t="s">
         <v>437</v>
       </c>
@@ -6884,7 +7013,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="164" ht="14.4" hidden="1" customHeight="1" spans="1:9">
+    <row r="164" ht="14.4" customHeight="1" spans="1:9">
       <c r="A164" t="s">
         <v>437</v>
       </c>
@@ -6911,7 +7040,7 @@
       </c>
       <c r="I164" s="8"/>
     </row>
-    <row r="165" ht="14.4" hidden="1" customHeight="1" spans="1:9">
+    <row r="165" ht="14.4" customHeight="1" spans="1:9">
       <c r="A165" t="s">
         <v>437</v>
       </c>
@@ -6969,11 +7098,6 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:XEX166">
-    <filterColumn colId="6">
-      <filters>
-        <filter val="1"/>
-      </filters>
-    </filterColumn>
     <extLst/>
   </autoFilter>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555556" footer="0.511805555555556"/>

</xml_diff>

<commit_message>
update level2 logfile b2c257e0-3ad7-4f05-b8e3-d9da973be36e
Signed-off-by: wangalexy <wangalexy@mailto.plus>
</commit_message>
<xml_diff>
--- a/results/GAIA/validation/gaia_validation.xlsx
+++ b/results/GAIA/validation/gaia_validation.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1034" uniqueCount="551">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1035" uniqueCount="551">
   <si>
     <t>Level</t>
   </si>
@@ -2796,7 +2796,7 @@
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="J43" sqref="J43"/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10" defaultRowHeight="15.6"/>
@@ -4264,14 +4264,14 @@
       <c r="D57" t="s">
         <v>184</v>
       </c>
-      <c r="E57">
-        <v>-23.6</v>
+      <c r="E57" t="s">
+        <v>184</v>
       </c>
       <c r="G57">
         <v>1</v>
       </c>
       <c r="I57">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="58" ht="14.4" customHeight="1" spans="1:9">

</xml_diff>

<commit_message>
update level1 logfile 50ad0280-0819-4bd9-b275-5de32d3b5bcb
Signed-off-by: wangalexy <wangalexy@mailto.plus>
</commit_message>
<xml_diff>
--- a/results/GAIA/validation/gaia_validation.xlsx
+++ b/results/GAIA/validation/gaia_validation.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1035" uniqueCount="551">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1036" uniqueCount="551">
   <si>
     <t>Level</t>
   </si>
@@ -3795,7 +3795,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="39" ht="14.4" spans="1:9">
+    <row r="39" spans="1:9">
       <c r="A39" t="s">
         <v>9</v>
       </c>
@@ -3817,7 +3817,9 @@
       <c r="G39">
         <v>1</v>
       </c>
-      <c r="I39" s="8"/>
+      <c r="I39" s="8" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="40" ht="14.4" spans="1:9">
       <c r="A40" t="s">

</xml_diff>

<commit_message>
update level1 logfile 1f975693-876d-457b-a649-393859e79bf3
Signed-off-by: wangalexy <wangalexy@mailto.plus>
</commit_message>
<xml_diff>
--- a/results/GAIA/validation/gaia_validation.xlsx
+++ b/results/GAIA/validation/gaia_validation.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1036" uniqueCount="551">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1037" uniqueCount="552">
   <si>
     <t>Level</t>
   </si>
@@ -506,6 +506,9 @@
   </si>
   <si>
     <t>132, 133, 134, 197, 245</t>
+  </si>
+  <si>
+    <t>132,133,134,197,245</t>
   </si>
   <si>
     <t>840bfca7-4f7b-481a-8794-c560c340185d</t>
@@ -2438,11 +2441,11 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="47" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
@@ -2796,7 +2799,7 @@
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="I51" sqref="I51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10" defaultRowHeight="15.6"/>
@@ -2838,7 +2841,7 @@
       <c r="H1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="I1" s="8" t="s">
         <v>8</v>
       </c>
     </row>
@@ -2864,7 +2867,7 @@
       <c r="G2">
         <v>1</v>
       </c>
-      <c r="I2" s="8">
+      <c r="I2" s="6">
         <v>1</v>
       </c>
     </row>
@@ -2890,7 +2893,7 @@
       <c r="G3">
         <v>1</v>
       </c>
-      <c r="I3" s="8">
+      <c r="I3" s="6">
         <v>1</v>
       </c>
     </row>
@@ -2916,7 +2919,7 @@
       <c r="G4">
         <v>1</v>
       </c>
-      <c r="I4" s="8">
+      <c r="I4" s="6">
         <v>1</v>
       </c>
     </row>
@@ -2942,7 +2945,7 @@
       <c r="G5">
         <v>1</v>
       </c>
-      <c r="I5" s="8">
+      <c r="I5" s="6">
         <v>1</v>
       </c>
     </row>
@@ -2965,7 +2968,7 @@
       <c r="G6">
         <v>1</v>
       </c>
-      <c r="I6" s="8">
+      <c r="I6" s="6">
         <v>1</v>
       </c>
     </row>
@@ -2991,7 +2994,7 @@
       <c r="G7">
         <v>1</v>
       </c>
-      <c r="I7" s="8">
+      <c r="I7" s="6">
         <v>1</v>
       </c>
     </row>
@@ -3017,7 +3020,7 @@
       <c r="G8">
         <v>1</v>
       </c>
-      <c r="I8" s="8" t="s">
+      <c r="I8" s="6" t="s">
         <v>30</v>
       </c>
     </row>
@@ -3043,7 +3046,7 @@
       <c r="G9">
         <v>1</v>
       </c>
-      <c r="I9" s="8" t="s">
+      <c r="I9" s="6" t="s">
         <v>30</v>
       </c>
     </row>
@@ -3069,7 +3072,7 @@
       <c r="G10">
         <v>1</v>
       </c>
-      <c r="I10" s="8">
+      <c r="I10" s="6">
         <v>1</v>
       </c>
     </row>
@@ -3095,7 +3098,7 @@
       <c r="G11">
         <v>1</v>
       </c>
-      <c r="I11" s="8">
+      <c r="I11" s="6">
         <v>1</v>
       </c>
     </row>
@@ -3121,7 +3124,7 @@
       <c r="G12">
         <v>1</v>
       </c>
-      <c r="I12" s="8">
+      <c r="I12" s="6">
         <v>1</v>
       </c>
     </row>
@@ -3147,7 +3150,7 @@
       <c r="G13">
         <v>1</v>
       </c>
-      <c r="I13" s="8">
+      <c r="I13" s="6">
         <v>1</v>
       </c>
     </row>
@@ -3173,7 +3176,7 @@
       <c r="G14">
         <v>1</v>
       </c>
-      <c r="I14" s="8">
+      <c r="I14" s="6">
         <v>1</v>
       </c>
     </row>
@@ -3199,7 +3202,7 @@
       <c r="G15">
         <v>1</v>
       </c>
-      <c r="I15" s="8" t="s">
+      <c r="I15" s="6" t="s">
         <v>30</v>
       </c>
     </row>
@@ -3225,7 +3228,7 @@
       <c r="G16">
         <v>1</v>
       </c>
-      <c r="I16" s="8">
+      <c r="I16" s="6">
         <v>1</v>
       </c>
     </row>
@@ -3251,7 +3254,7 @@
       <c r="G17">
         <v>0</v>
       </c>
-      <c r="I17" s="8"/>
+      <c r="I17" s="6"/>
     </row>
     <row r="18" ht="14.4" spans="1:9">
       <c r="A18" t="s">
@@ -3275,7 +3278,7 @@
       <c r="G18">
         <v>0</v>
       </c>
-      <c r="I18" s="8"/>
+      <c r="I18" s="6"/>
     </row>
     <row r="19" ht="14.4" spans="1:9">
       <c r="A19" t="s">
@@ -3299,7 +3302,7 @@
       <c r="G19">
         <v>1</v>
       </c>
-      <c r="I19" s="8" t="s">
+      <c r="I19" s="6" t="s">
         <v>30</v>
       </c>
     </row>
@@ -3325,7 +3328,7 @@
       <c r="G20">
         <v>1</v>
       </c>
-      <c r="I20" s="8" t="s">
+      <c r="I20" s="6" t="s">
         <v>30</v>
       </c>
     </row>
@@ -3351,7 +3354,7 @@
       <c r="G21">
         <v>1</v>
       </c>
-      <c r="I21" s="8" t="s">
+      <c r="I21" s="6" t="s">
         <v>30</v>
       </c>
     </row>
@@ -3377,7 +3380,7 @@
       <c r="G22">
         <v>1</v>
       </c>
-      <c r="I22" s="8" t="s">
+      <c r="I22" s="6" t="s">
         <v>30</v>
       </c>
     </row>
@@ -3403,7 +3406,7 @@
       <c r="G23">
         <v>0</v>
       </c>
-      <c r="I23" s="8"/>
+      <c r="I23" s="6"/>
     </row>
     <row r="24" ht="14.4" spans="1:9">
       <c r="A24" t="s">
@@ -3427,7 +3430,7 @@
       <c r="G24">
         <v>1</v>
       </c>
-      <c r="I24" s="8" t="s">
+      <c r="I24" s="6" t="s">
         <v>30</v>
       </c>
     </row>
@@ -3453,7 +3456,7 @@
       <c r="G25">
         <v>1</v>
       </c>
-      <c r="I25" s="8" t="s">
+      <c r="I25" s="6" t="s">
         <v>30</v>
       </c>
     </row>
@@ -3479,7 +3482,7 @@
       <c r="G26">
         <v>1</v>
       </c>
-      <c r="I26" s="8" t="s">
+      <c r="I26" s="6" t="s">
         <v>30</v>
       </c>
     </row>
@@ -3505,7 +3508,7 @@
       <c r="G27">
         <v>1</v>
       </c>
-      <c r="I27" s="8" t="s">
+      <c r="I27" s="6" t="s">
         <v>30</v>
       </c>
     </row>
@@ -3531,7 +3534,7 @@
       <c r="G28">
         <v>1</v>
       </c>
-      <c r="I28" s="8" t="s">
+      <c r="I28" s="6" t="s">
         <v>30</v>
       </c>
     </row>
@@ -3557,7 +3560,7 @@
       <c r="G29">
         <v>1</v>
       </c>
-      <c r="I29" s="8" t="s">
+      <c r="I29" s="6" t="s">
         <v>30</v>
       </c>
     </row>
@@ -3583,7 +3586,7 @@
       <c r="G30">
         <v>1</v>
       </c>
-      <c r="I30" s="8" t="s">
+      <c r="I30" s="6" t="s">
         <v>30</v>
       </c>
     </row>
@@ -3609,7 +3612,7 @@
       <c r="G31">
         <v>1</v>
       </c>
-      <c r="I31" s="8" t="s">
+      <c r="I31" s="6" t="s">
         <v>30</v>
       </c>
     </row>
@@ -3635,7 +3638,7 @@
       <c r="G32">
         <v>1</v>
       </c>
-      <c r="I32" s="8" t="s">
+      <c r="I32" s="6" t="s">
         <v>30</v>
       </c>
     </row>
@@ -3661,7 +3664,7 @@
       <c r="G33">
         <v>1</v>
       </c>
-      <c r="I33" s="8" t="s">
+      <c r="I33" s="6" t="s">
         <v>30</v>
       </c>
     </row>
@@ -3687,7 +3690,7 @@
       <c r="G34">
         <v>1</v>
       </c>
-      <c r="I34" s="8" t="s">
+      <c r="I34" s="6" t="s">
         <v>30</v>
       </c>
     </row>
@@ -3713,7 +3716,7 @@
       <c r="G35">
         <v>1</v>
       </c>
-      <c r="I35" s="8" t="s">
+      <c r="I35" s="6" t="s">
         <v>30</v>
       </c>
     </row>
@@ -3739,7 +3742,7 @@
       <c r="G36">
         <v>1</v>
       </c>
-      <c r="I36" s="8" t="s">
+      <c r="I36" s="6" t="s">
         <v>30</v>
       </c>
     </row>
@@ -3765,7 +3768,7 @@
       <c r="G37">
         <v>1</v>
       </c>
-      <c r="I37" s="8" t="s">
+      <c r="I37" s="6" t="s">
         <v>30</v>
       </c>
     </row>
@@ -3791,11 +3794,11 @@
       <c r="G38">
         <v>1</v>
       </c>
-      <c r="I38" s="8" t="s">
+      <c r="I38" s="6" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="39" spans="1:9">
+    <row r="39" ht="14.4" spans="1:9">
       <c r="A39" t="s">
         <v>9</v>
       </c>
@@ -3817,7 +3820,7 @@
       <c r="G39">
         <v>1</v>
       </c>
-      <c r="I39" s="8" t="s">
+      <c r="I39" s="6" t="s">
         <v>30</v>
       </c>
     </row>
@@ -3843,7 +3846,7 @@
       <c r="G40">
         <v>0</v>
       </c>
-      <c r="I40" s="8"/>
+      <c r="I40" s="6"/>
     </row>
     <row r="41" ht="14.4" spans="1:9">
       <c r="A41" t="s">
@@ -3867,7 +3870,7 @@
       <c r="G41">
         <v>1</v>
       </c>
-      <c r="I41" s="8"/>
+      <c r="I41" s="6"/>
     </row>
     <row r="42" ht="14.4" spans="1:9">
       <c r="A42" t="s">
@@ -3891,7 +3894,7 @@
       <c r="G42">
         <v>1</v>
       </c>
-      <c r="I42" s="8" t="s">
+      <c r="I42" s="6" t="s">
         <v>30</v>
       </c>
     </row>
@@ -3917,7 +3920,7 @@
       <c r="G43">
         <v>1</v>
       </c>
-      <c r="I43" s="8" t="s">
+      <c r="I43" s="6" t="s">
         <v>30</v>
       </c>
     </row>
@@ -3943,7 +3946,7 @@
       <c r="G44">
         <v>1</v>
       </c>
-      <c r="I44" s="8" t="s">
+      <c r="I44" s="6" t="s">
         <v>30</v>
       </c>
     </row>
@@ -3969,7 +3972,7 @@
       <c r="G45">
         <v>1</v>
       </c>
-      <c r="I45" s="8" t="s">
+      <c r="I45" s="6" t="s">
         <v>30</v>
       </c>
     </row>
@@ -3986,8 +3989,8 @@
       <c r="D46" t="s">
         <v>148</v>
       </c>
-      <c r="E46" t="s">
-        <v>148</v>
+      <c r="E46" s="6" t="s">
+        <v>149</v>
       </c>
       <c r="F46" t="s">
         <v>13</v>
@@ -3995,23 +3998,25 @@
       <c r="G46">
         <v>1</v>
       </c>
-      <c r="I46" s="8"/>
+      <c r="I46" s="6" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="47" ht="14.4" spans="1:9">
       <c r="A47" t="s">
         <v>9</v>
       </c>
       <c r="B47" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C47" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="D47" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="E47" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="F47" t="s">
         <v>13</v>
@@ -4019,7 +4024,7 @@
       <c r="G47">
         <v>1</v>
       </c>
-      <c r="I47" s="8" t="s">
+      <c r="I47" s="6" t="s">
         <v>30</v>
       </c>
     </row>
@@ -4028,13 +4033,13 @@
         <v>9</v>
       </c>
       <c r="B48" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C48" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="D48" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="E48">
         <v>90</v>
@@ -4045,7 +4050,7 @@
       <c r="G48">
         <v>1</v>
       </c>
-      <c r="I48" s="8" t="s">
+      <c r="I48" s="6" t="s">
         <v>30</v>
       </c>
     </row>
@@ -4054,16 +4059,16 @@
         <v>9</v>
       </c>
       <c r="B49" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="C49" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="D49" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="E49" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="F49" t="s">
         <v>13</v>
@@ -4071,7 +4076,7 @@
       <c r="G49">
         <v>1</v>
       </c>
-      <c r="I49" s="8" t="s">
+      <c r="I49" s="6" t="s">
         <v>30</v>
       </c>
     </row>
@@ -4080,16 +4085,16 @@
         <v>9</v>
       </c>
       <c r="B50" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="C50" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="D50" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="E50" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="F50" t="s">
         <v>13</v>
@@ -4097,7 +4102,7 @@
       <c r="G50">
         <v>1</v>
       </c>
-      <c r="I50" s="8" t="s">
+      <c r="I50" s="6" t="s">
         <v>30</v>
       </c>
     </row>
@@ -4106,16 +4111,16 @@
         <v>9</v>
       </c>
       <c r="B51" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C51" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="D51" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="E51" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="F51" t="s">
         <v>13</v>
@@ -4123,23 +4128,23 @@
       <c r="G51">
         <v>1</v>
       </c>
-      <c r="I51" s="8"/>
+      <c r="I51" s="6"/>
     </row>
     <row r="52" ht="14.4" spans="1:9">
       <c r="A52" t="s">
         <v>9</v>
       </c>
       <c r="B52" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C52" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="D52" t="s">
-        <v>167</v>
-      </c>
-      <c r="E52" s="6" t="s">
         <v>168</v>
+      </c>
+      <c r="E52" s="7" t="s">
+        <v>169</v>
       </c>
       <c r="F52" t="s">
         <v>13</v>
@@ -4147,23 +4152,23 @@
       <c r="G52">
         <v>0</v>
       </c>
-      <c r="I52" s="8"/>
+      <c r="I52" s="6"/>
     </row>
     <row r="53" ht="14.4" spans="1:9">
       <c r="A53" t="s">
         <v>9</v>
       </c>
       <c r="B53" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="C53" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="D53" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="E53" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="F53" t="s">
         <v>13</v>
@@ -4171,7 +4176,7 @@
       <c r="G53">
         <v>1</v>
       </c>
-      <c r="I53" s="8" t="s">
+      <c r="I53" s="6" t="s">
         <v>30</v>
       </c>
     </row>
@@ -4180,16 +4185,16 @@
         <v>9</v>
       </c>
       <c r="B54" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C54" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="D54" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="E54" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="F54" t="s">
         <v>13</v>
@@ -4197,25 +4202,25 @@
       <c r="G54">
         <v>1</v>
       </c>
-      <c r="I54" s="8" t="s">
+      <c r="I54" s="6" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="55" ht="14.4" customHeight="1" spans="1:9">
       <c r="A55" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B55" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C55" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="D55" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="E55" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="F55" t="s">
         <v>13</v>
@@ -4229,19 +4234,19 @@
     </row>
     <row r="56" ht="14.4" customHeight="1" spans="1:9">
       <c r="A56" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B56" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="C56" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="D56" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="E56" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="F56" t="s">
         <v>13</v>
@@ -4255,19 +4260,19 @@
     </row>
     <row r="57" ht="14.4" customHeight="1" spans="1:9">
       <c r="A57" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B57" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="C57" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="D57" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="E57" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="G57">
         <v>1</v>
@@ -4278,16 +4283,16 @@
     </row>
     <row r="58" ht="14.4" customHeight="1" spans="1:9">
       <c r="A58" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B58" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="C58" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="D58" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="E58">
         <v>10</v>
@@ -4301,19 +4306,19 @@
     </row>
     <row r="59" ht="14.4" customHeight="1" spans="1:9">
       <c r="A59" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B59" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="C59" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="D59" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="E59" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="F59" t="s">
         <v>13</v>
@@ -4327,19 +4332,19 @@
     </row>
     <row r="60" ht="14.4" customHeight="1" spans="1:9">
       <c r="A60" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B60" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="C60" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="D60" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="E60" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="F60" t="s">
         <v>13</v>
@@ -4353,19 +4358,19 @@
     </row>
     <row r="61" ht="14.4" customHeight="1" spans="1:9">
       <c r="A61" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B61" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="C61" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="D61" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="E61" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="F61" t="s">
         <v>13</v>
@@ -4379,13 +4384,13 @@
     </row>
     <row r="62" ht="14.4" customHeight="1" spans="1:9">
       <c r="A62" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B62" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C62" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="D62" t="s">
         <v>120</v>
@@ -4405,19 +4410,19 @@
     </row>
     <row r="63" ht="14.4" customHeight="1" spans="1:9">
       <c r="A63" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B63" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="C63" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="D63" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="E63" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="F63" t="s">
         <v>13</v>
@@ -4431,19 +4436,19 @@
     </row>
     <row r="64" ht="14.4" customHeight="1" spans="1:9">
       <c r="A64" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B64" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="C64" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="D64" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="E64" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="F64" t="s">
         <v>13</v>
@@ -4457,19 +4462,19 @@
     </row>
     <row r="65" ht="14.4" customHeight="1" spans="1:9">
       <c r="A65" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B65" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="C65" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="D65" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="E65" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="F65" t="s">
         <v>13</v>
@@ -4483,19 +4488,19 @@
     </row>
     <row r="66" ht="14.4" customHeight="1" spans="1:9">
       <c r="A66" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B66" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="C66" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="D66" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="E66" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="F66" t="s">
         <v>13</v>
@@ -4509,16 +4514,16 @@
     </row>
     <row r="67" ht="14.4" customHeight="1" spans="1:9">
       <c r="A67" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B67" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="C67" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="D67" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="E67">
         <v>16.094</v>
@@ -4535,19 +4540,19 @@
     </row>
     <row r="68" ht="14.4" customHeight="1" spans="1:9">
       <c r="A68" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B68" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="C68" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="D68" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="E68" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="F68" t="s">
         <v>13</v>
@@ -4561,19 +4566,19 @@
     </row>
     <row r="69" ht="14.4" customHeight="1" spans="1:9">
       <c r="A69" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B69" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="C69" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="D69" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="E69" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="F69" t="s">
         <v>13</v>
@@ -4587,19 +4592,19 @@
     </row>
     <row r="70" ht="14.4" customHeight="1" spans="1:9">
       <c r="A70" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B70" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="C70" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="D70" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="E70" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="F70" t="s">
         <v>13</v>
@@ -4613,16 +4618,16 @@
     </row>
     <row r="71" ht="14.4" customHeight="1" spans="1:9">
       <c r="A71" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B71" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="C71" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="D71" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="E71">
         <v>9</v>
@@ -4639,19 +4644,19 @@
     </row>
     <row r="72" ht="14.4" customHeight="1" spans="1:9">
       <c r="A72" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B72" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="C72" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="D72" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="E72" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="F72" t="s">
         <v>13</v>
@@ -4665,16 +4670,16 @@
     </row>
     <row r="73" ht="14.4" customHeight="1" spans="1:9">
       <c r="A73" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B73" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="C73" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="D73" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="E73">
         <v>52</v>
@@ -4691,13 +4696,13 @@
     </row>
     <row r="74" ht="14.4" customHeight="1" spans="1:9">
       <c r="A74" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B74" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="C74" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="D74" t="s">
         <v>12</v>
@@ -4717,19 +4722,19 @@
     </row>
     <row r="75" ht="14.4" customHeight="1" spans="1:9">
       <c r="A75" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B75" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="C75" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="D75" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="E75" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="F75" t="s">
         <v>13</v>
@@ -4743,19 +4748,19 @@
     </row>
     <row r="76" ht="14.4" customHeight="1" spans="1:9">
       <c r="A76" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B76" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="C76" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="D76" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="E76" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="F76" t="s">
         <v>13</v>
@@ -4769,13 +4774,13 @@
     </row>
     <row r="77" ht="14.4" customHeight="1" spans="1:9">
       <c r="A77" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B77" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C77" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="D77" t="s">
         <v>16</v>
@@ -4792,19 +4797,19 @@
     </row>
     <row r="78" ht="14.4" customHeight="1" spans="1:9">
       <c r="A78" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B78" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="C78" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="D78" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="E78" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="F78" t="s">
         <v>13</v>
@@ -4818,13 +4823,13 @@
     </row>
     <row r="79" ht="14.4" customHeight="1" spans="1:9">
       <c r="A79" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B79" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="C79" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="D79" t="s">
         <v>16</v>
@@ -4844,16 +4849,16 @@
     </row>
     <row r="80" ht="14.4" customHeight="1" spans="1:9">
       <c r="A80" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B80" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="C80" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="D80" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="E80" s="9">
         <v>0.711805555555556</v>
@@ -4870,19 +4875,19 @@
     </row>
     <row r="81" ht="14.4" customHeight="1" spans="1:9">
       <c r="A81" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B81" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="C81" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="D81" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="E81" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="G81">
         <v>1</v>
@@ -4893,19 +4898,19 @@
     </row>
     <row r="82" ht="14.4" customHeight="1" spans="1:9">
       <c r="A82" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B82" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="C82" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="D82" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="E82" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="G82">
         <v>1</v>
@@ -4916,19 +4921,19 @@
     </row>
     <row r="83" ht="14.4" customHeight="1" spans="1:9">
       <c r="A83" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B83" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="C83" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="D83" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="E83" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="G83">
         <v>1</v>
@@ -4939,19 +4944,19 @@
     </row>
     <row r="84" ht="14.4" customHeight="1" spans="1:9">
       <c r="A84" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B84" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="C84" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="D84" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="E84" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="F84" t="s">
         <v>13</v>
@@ -4965,19 +4970,19 @@
     </row>
     <row r="85" ht="14.4" customHeight="1" spans="1:9">
       <c r="A85" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B85" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="C85" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="D85" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="E85" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="F85" t="s">
         <v>13</v>
@@ -4991,16 +4996,16 @@
     </row>
     <row r="86" ht="14.4" customHeight="1" spans="1:9">
       <c r="A86" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B86" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="C86" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="D86" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="E86">
         <v>41</v>
@@ -5017,13 +5022,13 @@
     </row>
     <row r="87" ht="14.4" customHeight="1" spans="1:9">
       <c r="A87" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B87" s="10" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="C87" s="10" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="D87" s="10" t="s">
         <v>120</v>
@@ -5044,19 +5049,19 @@
     </row>
     <row r="88" ht="14.4" customHeight="1" spans="1:9">
       <c r="A88" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B88" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="C88" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="D88" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="E88" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="F88" t="s">
         <v>13</v>
@@ -5070,19 +5075,19 @@
     </row>
     <row r="89" ht="14.4" customHeight="1" spans="1:9">
       <c r="A89" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B89" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="C89" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="D89" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="E89" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="F89" t="s">
         <v>13</v>
@@ -5096,19 +5101,19 @@
     </row>
     <row r="90" ht="14.4" customHeight="1" spans="1:9">
       <c r="A90" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B90" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="C90" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="D90" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="E90" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="F90" t="s">
         <v>13</v>
@@ -5122,19 +5127,19 @@
     </row>
     <row r="91" ht="14.4" customHeight="1" spans="1:9">
       <c r="A91" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B91" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="C91" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D91" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="E91" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="F91" t="s">
         <v>13</v>
@@ -5148,13 +5153,13 @@
     </row>
     <row r="92" ht="14.4" customHeight="1" spans="1:9">
       <c r="A92" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B92" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="C92" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="D92" t="s">
         <v>45</v>
@@ -5174,19 +5179,19 @@
     </row>
     <row r="93" ht="14.4" customHeight="1" spans="1:7">
       <c r="A93" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B93" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="C93" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="D93" t="s">
         <v>87</v>
       </c>
       <c r="E93" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="F93" t="s">
         <v>13</v>
@@ -5197,19 +5202,19 @@
     </row>
     <row r="94" ht="14.4" customHeight="1" spans="1:7">
       <c r="A94" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B94" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="C94" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="D94" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="E94" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="F94" t="s">
         <v>13</v>
@@ -5220,19 +5225,19 @@
     </row>
     <row r="95" ht="14.4" customHeight="1" spans="1:9">
       <c r="A95" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B95" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="C95" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="D95" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="E95" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="F95" t="s">
         <v>13</v>
@@ -5246,19 +5251,19 @@
     </row>
     <row r="96" ht="14.4" customHeight="1" spans="1:9">
       <c r="A96" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B96" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="C96" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="D96" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="E96" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="F96" t="s">
         <v>13</v>
@@ -5272,19 +5277,19 @@
     </row>
     <row r="97" ht="14.4" customHeight="1" spans="1:9">
       <c r="A97" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B97" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="C97" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="D97" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="E97" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="F97" t="s">
         <v>13</v>
@@ -5298,13 +5303,13 @@
     </row>
     <row r="98" ht="14.4" customHeight="1" spans="1:9">
       <c r="A98" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B98" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="C98" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="D98" t="s">
         <v>120</v>
@@ -5324,16 +5329,16 @@
     </row>
     <row r="99" ht="14.4" customHeight="1" spans="1:7">
       <c r="A99" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B99" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="C99" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="D99" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="E99">
         <v>126</v>
@@ -5347,19 +5352,19 @@
     </row>
     <row r="100" ht="14.4" customHeight="1" spans="1:9">
       <c r="A100" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B100" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="C100" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="D100" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="E100" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="F100" t="s">
         <v>13</v>
@@ -5373,16 +5378,16 @@
     </row>
     <row r="101" ht="14.4" customHeight="1" spans="1:7">
       <c r="A101" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B101" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="C101" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="D101" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="E101">
         <v>2018</v>
@@ -5396,13 +5401,13 @@
     </row>
     <row r="102" ht="14.4" customHeight="1" spans="1:9">
       <c r="A102" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B102" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="C102" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="D102" t="s">
         <v>117</v>
@@ -5422,19 +5427,19 @@
     </row>
     <row r="103" ht="14.4" customHeight="1" spans="1:7">
       <c r="A103" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B103" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="C103" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="D103" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="E103" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="F103" t="s">
         <v>13</v>
@@ -5445,16 +5450,16 @@
     </row>
     <row r="104" ht="14.4" customHeight="1" spans="1:7">
       <c r="A104" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B104" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="C104" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="D104" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="E104">
         <v>90</v>
@@ -5468,16 +5473,16 @@
     </row>
     <row r="105" ht="14.4" customHeight="1" spans="1:7">
       <c r="A105" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B105" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="C105" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="D105" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="E105">
         <v>13</v>
@@ -5491,16 +5496,16 @@
     </row>
     <row r="106" ht="14.4" customHeight="1" spans="1:9">
       <c r="A106" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B106" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="C106" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="D106" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="E106">
         <v>7</v>
@@ -5517,19 +5522,19 @@
     </row>
     <row r="107" ht="14.4" customHeight="1" spans="1:9">
       <c r="A107" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B107" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="C107" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="D107" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="E107" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="F107" t="s">
         <v>13</v>
@@ -5543,16 +5548,16 @@
     </row>
     <row r="108" ht="14.4" customHeight="1" spans="1:9">
       <c r="A108" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B108" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="C108" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="D108" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="E108">
         <v>860000</v>
@@ -5569,19 +5574,19 @@
     </row>
     <row r="109" ht="14.4" customHeight="1" spans="1:9">
       <c r="A109" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B109" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="C109" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="D109" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="E109" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="F109" t="s">
         <v>13</v>
@@ -5595,16 +5600,16 @@
     </row>
     <row r="110" ht="14.4" customHeight="1" spans="1:9">
       <c r="A110" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B110" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="C110" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="D110" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="E110">
         <v>563.9</v>
@@ -5621,19 +5626,19 @@
     </row>
     <row r="111" ht="14.4" customHeight="1" spans="1:9">
       <c r="A111" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B111" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="C111" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="D111" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="E111" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="F111" t="s">
         <v>13</v>
@@ -5647,19 +5652,19 @@
     </row>
     <row r="112" ht="14.4" customHeight="1" spans="1:9">
       <c r="A112" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B112" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="C112" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="D112" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="E112" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="F112" t="s">
         <v>13</v>
@@ -5673,19 +5678,19 @@
     </row>
     <row r="113" ht="14.4" customHeight="1" spans="1:9">
       <c r="A113" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B113" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="C113" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="D113" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="E113" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="F113" t="s">
         <v>13</v>
@@ -5699,19 +5704,19 @@
     </row>
     <row r="114" ht="14.4" customHeight="1" spans="1:9">
       <c r="A114" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B114" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="C114" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="D114" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="E114" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="F114" t="s">
         <v>13</v>
@@ -5725,13 +5730,13 @@
     </row>
     <row r="115" ht="14.4" customHeight="1" spans="1:9">
       <c r="A115" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B115" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="C115" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="D115" t="s">
         <v>45</v>
@@ -5751,16 +5756,16 @@
     </row>
     <row r="116" ht="14.4" customHeight="1" spans="1:7">
       <c r="A116" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B116" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="C116" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="D116" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="E116">
         <v>1785</v>
@@ -5774,13 +5779,13 @@
     </row>
     <row r="117" ht="14.4" customHeight="1" spans="1:7">
       <c r="A117" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B117" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="C117" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="D117" t="s">
         <v>87</v>
@@ -5797,16 +5802,16 @@
     </row>
     <row r="118" ht="14.4" customHeight="1" spans="1:7">
       <c r="A118" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B118" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="C118" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="D118" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="E118">
         <v>3</v>
@@ -5820,16 +5825,16 @@
     </row>
     <row r="119" ht="14.4" customHeight="1" spans="1:9">
       <c r="A119" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B119" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="C119" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="D119" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="E119">
         <v>60</v>
@@ -5846,19 +5851,19 @@
     </row>
     <row r="120" ht="14.4" customHeight="1" spans="1:9">
       <c r="A120" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B120" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="C120" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="D120" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="E120" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="F120" t="s">
         <v>13</v>
@@ -5872,19 +5877,19 @@
     </row>
     <row r="121" ht="14.4" customHeight="1" spans="1:9">
       <c r="A121" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B121" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="C121" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="D121" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="E121" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="F121" t="s">
         <v>13</v>
@@ -5898,19 +5903,19 @@
     </row>
     <row r="122" ht="14.4" customHeight="1" spans="1:9">
       <c r="A122" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B122" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="C122" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="D122" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="E122" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="F122" t="s">
         <v>13</v>
@@ -5924,19 +5929,19 @@
     </row>
     <row r="123" ht="14.4" customHeight="1" spans="1:9">
       <c r="A123" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B123" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="C123" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="D123" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="E123" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="F123" t="s">
         <v>13</v>
@@ -5950,16 +5955,16 @@
     </row>
     <row r="124" ht="14.4" customHeight="1" spans="1:9">
       <c r="A124" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B124" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="C124" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="D124" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="E124">
         <v>8</v>
@@ -5976,19 +5981,19 @@
     </row>
     <row r="125" ht="14.4" customHeight="1" spans="1:9">
       <c r="A125" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B125" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="C125" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="D125" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="E125" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="F125" t="s">
         <v>13</v>
@@ -6002,19 +6007,19 @@
     </row>
     <row r="126" ht="14.4" customHeight="1" spans="1:9">
       <c r="A126" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B126" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="C126" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="D126" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="E126" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="F126" t="s">
         <v>13</v>
@@ -6028,19 +6033,19 @@
     </row>
     <row r="127" ht="14.4" customHeight="1" spans="1:7">
       <c r="A127" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B127" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="C127" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D127" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="E127" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="F127" t="s">
         <v>13</v>
@@ -6051,16 +6056,16 @@
     </row>
     <row r="128" ht="14.4" customHeight="1" spans="1:9">
       <c r="A128" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B128" s="10" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="C128" s="10" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D128" s="10" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="E128" s="10">
         <v>477</v>
@@ -6076,19 +6081,19 @@
     </row>
     <row r="129" ht="14.4" customHeight="1" spans="1:9">
       <c r="A129" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B129" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="C129" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="D129" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="E129" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="F129" t="s">
         <v>13</v>
@@ -6102,19 +6107,19 @@
     </row>
     <row r="130" ht="14.4" customHeight="1" spans="1:9">
       <c r="A130" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B130" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="C130" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="D130" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="E130" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="F130" t="s">
         <v>13</v>
@@ -6128,16 +6133,16 @@
     </row>
     <row r="131" ht="14.4" customHeight="1" spans="1:9">
       <c r="A131" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B131" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="C131" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="D131" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="E131">
         <v>536</v>
@@ -6154,16 +6159,16 @@
     </row>
     <row r="132" ht="14.4" customHeight="1" spans="1:9">
       <c r="A132" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B132" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="C132" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="D132" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="E132">
         <v>1954</v>
@@ -6180,19 +6185,19 @@
     </row>
     <row r="133" ht="14.4" customHeight="1" spans="1:9">
       <c r="A133" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B133" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="C133" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="D133" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="E133" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="F133" t="s">
         <v>13</v>
@@ -6206,19 +6211,19 @@
     </row>
     <row r="134" ht="14.4" customHeight="1" spans="1:9">
       <c r="A134" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B134" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="C134" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="D134" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="E134" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="F134" t="s">
         <v>13</v>
@@ -6232,19 +6237,19 @@
     </row>
     <row r="135" ht="14.4" customHeight="1" spans="1:9">
       <c r="A135" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B135" s="10" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="C135" s="10" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="D135" s="10" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="E135" s="10" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="F135" s="10" t="s">
         <v>13</v>
@@ -6259,16 +6264,16 @@
     </row>
     <row r="136" ht="14.4" customHeight="1" spans="1:9">
       <c r="A136" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B136" s="10" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="C136" s="10" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="D136" s="10" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="E136" s="10">
         <v>116</v>
@@ -6286,19 +6291,19 @@
     </row>
     <row r="137" ht="14.4" customHeight="1" spans="1:9">
       <c r="A137" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B137" s="10" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="C137" s="10" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="D137" s="10" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="E137" s="10" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="F137" s="10" t="s">
         <v>13</v>
@@ -6313,19 +6318,19 @@
     </row>
     <row r="138" ht="14.4" customHeight="1" spans="1:9">
       <c r="A138" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B138" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="C138" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="D138" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="E138" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="F138" t="s">
         <v>13</v>
@@ -6339,19 +6344,19 @@
     </row>
     <row r="139" ht="14.4" customHeight="1" spans="1:9">
       <c r="A139" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B139" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="C139" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="D139" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="E139" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="G139">
         <v>1</v>
@@ -6362,22 +6367,22 @@
     </row>
     <row r="140" ht="14.4" customHeight="1" spans="1:7">
       <c r="A140" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B140" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="C140" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="D140" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="E140" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="F140" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="G140">
         <v>0</v>
@@ -6385,19 +6390,19 @@
     </row>
     <row r="141" ht="14.4" customHeight="1" spans="1:9">
       <c r="A141" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="B141" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="C141" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="D141" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="E141" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="F141" t="s">
         <v>13</v>
@@ -6406,25 +6411,25 @@
         <v>0</v>
       </c>
       <c r="H141" t="s">
-        <v>442</v>
-      </c>
-      <c r="I141" s="8"/>
+        <v>443</v>
+      </c>
+      <c r="I141" s="6"/>
     </row>
     <row r="142" ht="14.4" customHeight="1" spans="1:9">
       <c r="A142" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="B142" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="C142" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="D142" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="E142" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="F142" t="s">
         <v>13</v>
@@ -6433,51 +6438,51 @@
         <v>0</v>
       </c>
       <c r="H142" t="s">
-        <v>447</v>
-      </c>
-      <c r="I142" s="8"/>
+        <v>448</v>
+      </c>
+      <c r="I142" s="6"/>
     </row>
     <row r="143" ht="14.4" customHeight="1" spans="1:9">
       <c r="A143" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="B143" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="C143" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="D143" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="E143" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="G143">
         <v>1</v>
       </c>
-      <c r="H143" s="6">
+      <c r="H143" s="7">
         <v>0.0368205208333333</v>
       </c>
-      <c r="I143" s="8">
+      <c r="I143" s="6">
         <v>1</v>
       </c>
     </row>
     <row r="144" ht="14.4" customHeight="1" spans="1:9">
       <c r="A144" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="B144" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="C144" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="D144" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="E144" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="F144" t="s">
         <v>13</v>
@@ -6486,25 +6491,25 @@
         <v>0</v>
       </c>
       <c r="H144" t="s">
-        <v>455</v>
-      </c>
-      <c r="I144" s="8"/>
+        <v>456</v>
+      </c>
+      <c r="I144" s="6"/>
     </row>
     <row r="145" ht="14.4" customHeight="1" spans="1:9">
       <c r="A145" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="B145" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="C145" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="D145" t="s">
         <v>137</v>
       </c>
       <c r="E145" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
       <c r="F145" t="s">
         <v>13</v>
@@ -6513,25 +6518,25 @@
         <v>0</v>
       </c>
       <c r="H145" t="s">
-        <v>459</v>
-      </c>
-      <c r="I145" s="8"/>
+        <v>460</v>
+      </c>
+      <c r="I145" s="6"/>
     </row>
     <row r="146" ht="14.4" customHeight="1" spans="1:9">
       <c r="A146" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="B146" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="C146" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="D146" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="E146" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="F146" t="s">
         <v>13</v>
@@ -6540,27 +6545,27 @@
         <v>1</v>
       </c>
       <c r="H146" t="s">
-        <v>463</v>
-      </c>
-      <c r="I146" s="8">
+        <v>464</v>
+      </c>
+      <c r="I146" s="6">
         <v>1</v>
       </c>
     </row>
     <row r="147" ht="14.4" customHeight="1" spans="1:9">
       <c r="A147" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="B147" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="C147" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="D147" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="E147" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="F147" t="s">
         <v>13</v>
@@ -6569,27 +6574,27 @@
         <v>1</v>
       </c>
       <c r="H147" t="s">
-        <v>467</v>
-      </c>
-      <c r="I147" s="8">
+        <v>468</v>
+      </c>
+      <c r="I147" s="6">
         <v>1</v>
       </c>
     </row>
     <row r="148" ht="14.4" customHeight="1" spans="1:9">
       <c r="A148" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="B148" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="C148" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="D148" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="E148" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="F148" t="s">
         <v>13</v>
@@ -6598,27 +6603,27 @@
         <v>1</v>
       </c>
       <c r="H148" t="s">
-        <v>471</v>
-      </c>
-      <c r="I148" s="8">
+        <v>472</v>
+      </c>
+      <c r="I148" s="6">
         <v>1</v>
       </c>
     </row>
     <row r="149" ht="14.4" customHeight="1" spans="1:9">
       <c r="A149" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="B149" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="C149" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="D149" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="E149" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="F149" t="s">
         <v>13</v>
@@ -6627,22 +6632,22 @@
         <v>0</v>
       </c>
       <c r="H149" t="s">
-        <v>476</v>
-      </c>
-      <c r="I149" s="8"/>
+        <v>477</v>
+      </c>
+      <c r="I149" s="6"/>
     </row>
     <row r="150" ht="14.4" customHeight="1" spans="1:9">
       <c r="A150" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="B150" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="C150" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="D150" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="E150" t="s">
         <v>117</v>
@@ -6654,25 +6659,25 @@
         <v>0</v>
       </c>
       <c r="H150" t="s">
-        <v>480</v>
-      </c>
-      <c r="I150" s="8"/>
+        <v>481</v>
+      </c>
+      <c r="I150" s="6"/>
     </row>
     <row r="151" ht="14.4" customHeight="1" spans="1:9">
       <c r="A151" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="B151" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
       <c r="C151" t="s">
-        <v>482</v>
+        <v>483</v>
       </c>
       <c r="D151" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="E151" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="F151" t="s">
         <v>13</v>
@@ -6681,25 +6686,25 @@
         <v>0</v>
       </c>
       <c r="H151" t="s">
-        <v>485</v>
-      </c>
-      <c r="I151" s="8"/>
+        <v>486</v>
+      </c>
+      <c r="I151" s="6"/>
     </row>
     <row r="152" ht="14.4" customHeight="1" spans="1:9">
       <c r="A152" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="B152" t="s">
-        <v>486</v>
+        <v>487</v>
       </c>
       <c r="C152" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
       <c r="D152" t="s">
-        <v>488</v>
+        <v>489</v>
       </c>
       <c r="E152" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
       <c r="F152" t="s">
         <v>13</v>
@@ -6708,25 +6713,25 @@
         <v>0</v>
       </c>
       <c r="H152" t="s">
-        <v>490</v>
-      </c>
-      <c r="I152" s="8"/>
+        <v>491</v>
+      </c>
+      <c r="I152" s="6"/>
     </row>
     <row r="153" ht="14.4" customHeight="1" spans="1:9">
       <c r="A153" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="B153" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="C153" t="s">
-        <v>492</v>
+        <v>493</v>
       </c>
       <c r="D153" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
       <c r="E153" t="s">
-        <v>494</v>
+        <v>495</v>
       </c>
       <c r="F153" t="s">
         <v>13</v>
@@ -6735,25 +6740,25 @@
         <v>0</v>
       </c>
       <c r="H153" t="s">
-        <v>495</v>
-      </c>
-      <c r="I153" s="8"/>
+        <v>496</v>
+      </c>
+      <c r="I153" s="6"/>
     </row>
     <row r="154" ht="14.4" customHeight="1" spans="1:9">
       <c r="A154" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="B154" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="C154" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="D154" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="E154" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
       <c r="F154" t="s">
         <v>13</v>
@@ -6762,25 +6767,25 @@
         <v>0</v>
       </c>
       <c r="H154" t="s">
-        <v>500</v>
-      </c>
-      <c r="I154" s="8"/>
+        <v>501</v>
+      </c>
+      <c r="I154" s="6"/>
     </row>
     <row r="155" ht="14.4" customHeight="1" spans="1:9">
       <c r="A155" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="B155" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C155" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="D155" t="s">
-        <v>503</v>
+        <v>504</v>
       </c>
       <c r="E155" t="s">
-        <v>503</v>
+        <v>504</v>
       </c>
       <c r="F155" t="s">
         <v>13</v>
@@ -6789,27 +6794,27 @@
         <v>1</v>
       </c>
       <c r="H155" t="s">
-        <v>504</v>
-      </c>
-      <c r="I155" s="8">
+        <v>505</v>
+      </c>
+      <c r="I155" s="6">
         <v>1</v>
       </c>
     </row>
     <row r="156" ht="14.4" customHeight="1" spans="1:9">
       <c r="A156" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="B156" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
       <c r="C156" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
       <c r="D156" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="E156" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="F156" t="s">
         <v>13</v>
@@ -6818,27 +6823,27 @@
         <v>1</v>
       </c>
       <c r="H156" t="s">
-        <v>508</v>
-      </c>
-      <c r="I156" s="8">
+        <v>509</v>
+      </c>
+      <c r="I156" s="6">
         <v>1</v>
       </c>
     </row>
     <row r="157" ht="14.4" customHeight="1" spans="1:9">
       <c r="A157" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="B157" t="s">
-        <v>509</v>
+        <v>510</v>
       </c>
       <c r="C157" t="s">
-        <v>510</v>
+        <v>511</v>
       </c>
       <c r="D157" t="s">
         <v>16</v>
       </c>
       <c r="E157" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
       <c r="F157" t="s">
         <v>13</v>
@@ -6847,25 +6852,25 @@
         <v>0</v>
       </c>
       <c r="H157" t="s">
-        <v>512</v>
-      </c>
-      <c r="I157" s="8"/>
+        <v>513</v>
+      </c>
+      <c r="I157" s="6"/>
     </row>
     <row r="158" ht="14.4" customHeight="1" spans="1:9">
       <c r="A158" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="B158" t="s">
-        <v>513</v>
+        <v>514</v>
       </c>
       <c r="C158" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="D158" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="E158" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
       <c r="F158" t="s">
         <v>13</v>
@@ -6874,24 +6879,24 @@
         <v>1</v>
       </c>
       <c r="H158" t="s">
-        <v>517</v>
-      </c>
-      <c r="I158" s="8">
+        <v>518</v>
+      </c>
+      <c r="I158" s="6">
         <v>1</v>
       </c>
     </row>
     <row r="159" ht="14.4" customHeight="1" spans="1:9">
       <c r="A159" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="B159" t="s">
-        <v>518</v>
+        <v>519</v>
       </c>
       <c r="C159" t="s">
-        <v>519</v>
+        <v>520</v>
       </c>
       <c r="D159" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="E159">
         <v>8</v>
@@ -6902,25 +6907,25 @@
       <c r="G159">
         <v>1</v>
       </c>
-      <c r="I159" s="8">
+      <c r="I159" s="6">
         <v>1</v>
       </c>
     </row>
     <row r="160" ht="14.4" customHeight="1" spans="1:9">
       <c r="A160" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="B160" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
       <c r="C160" t="s">
-        <v>521</v>
+        <v>522</v>
       </c>
       <c r="D160" t="s">
-        <v>522</v>
+        <v>523</v>
       </c>
       <c r="E160" t="s">
-        <v>522</v>
+        <v>523</v>
       </c>
       <c r="F160" t="s">
         <v>13</v>
@@ -6929,27 +6934,27 @@
         <v>1</v>
       </c>
       <c r="H160" t="s">
-        <v>523</v>
-      </c>
-      <c r="I160" s="8">
+        <v>524</v>
+      </c>
+      <c r="I160" s="6">
         <v>1</v>
       </c>
     </row>
     <row r="161" ht="14.4" customHeight="1" spans="1:9">
       <c r="A161" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="B161" t="s">
-        <v>524</v>
+        <v>525</v>
       </c>
       <c r="C161" t="s">
-        <v>525</v>
+        <v>526</v>
       </c>
       <c r="D161" t="s">
-        <v>526</v>
+        <v>527</v>
       </c>
       <c r="E161" t="s">
-        <v>527</v>
+        <v>528</v>
       </c>
       <c r="F161" t="s">
         <v>13</v>
@@ -6958,25 +6963,25 @@
         <v>0</v>
       </c>
       <c r="H161" t="s">
-        <v>528</v>
-      </c>
-      <c r="I161" s="8"/>
+        <v>529</v>
+      </c>
+      <c r="I161" s="6"/>
     </row>
     <row r="162" ht="14.4" customHeight="1" spans="1:9">
       <c r="A162" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="B162" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="C162" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
       <c r="D162" t="s">
-        <v>531</v>
+        <v>532</v>
       </c>
       <c r="E162" t="s">
-        <v>532</v>
+        <v>533</v>
       </c>
       <c r="F162" t="s">
         <v>13</v>
@@ -6985,25 +6990,25 @@
         <v>0</v>
       </c>
       <c r="H162" t="s">
-        <v>533</v>
-      </c>
-      <c r="I162" s="8"/>
+        <v>534</v>
+      </c>
+      <c r="I162" s="6"/>
     </row>
     <row r="163" ht="14.4" customHeight="1" spans="1:9">
       <c r="A163" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="B163" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="C163" t="s">
-        <v>535</v>
+        <v>536</v>
       </c>
       <c r="D163" t="s">
-        <v>536</v>
+        <v>537</v>
       </c>
       <c r="E163" t="s">
-        <v>536</v>
+        <v>537</v>
       </c>
       <c r="F163" t="s">
         <v>13</v>
@@ -7011,25 +7016,25 @@
       <c r="G163">
         <v>1</v>
       </c>
-      <c r="I163" s="8">
+      <c r="I163" s="6">
         <v>1</v>
       </c>
     </row>
     <row r="164" ht="14.4" customHeight="1" spans="1:9">
       <c r="A164" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="B164" t="s">
-        <v>537</v>
+        <v>538</v>
       </c>
       <c r="C164" t="s">
-        <v>538</v>
+        <v>539</v>
       </c>
       <c r="D164" t="s">
-        <v>539</v>
+        <v>540</v>
       </c>
       <c r="E164" t="s">
-        <v>540</v>
+        <v>541</v>
       </c>
       <c r="F164" t="s">
         <v>13</v>
@@ -7038,25 +7043,25 @@
         <v>0</v>
       </c>
       <c r="H164" t="s">
-        <v>541</v>
-      </c>
-      <c r="I164" s="8"/>
+        <v>542</v>
+      </c>
+      <c r="I164" s="6"/>
     </row>
     <row r="165" ht="14.4" customHeight="1" spans="1:9">
       <c r="A165" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="B165" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
       <c r="C165" t="s">
-        <v>543</v>
+        <v>544</v>
       </c>
       <c r="D165" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="E165" t="s">
-        <v>545</v>
+        <v>546</v>
       </c>
       <c r="F165" t="s">
         <v>13</v>
@@ -7065,25 +7070,25 @@
         <v>0</v>
       </c>
       <c r="H165" t="s">
-        <v>546</v>
-      </c>
-      <c r="I165" s="8"/>
+        <v>547</v>
+      </c>
+      <c r="I165" s="6"/>
     </row>
     <row r="166" ht="14.4" customHeight="1" spans="1:9">
       <c r="A166" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="B166" t="s">
-        <v>547</v>
+        <v>548</v>
       </c>
       <c r="C166" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
       <c r="D166" t="s">
-        <v>549</v>
+        <v>550</v>
       </c>
       <c r="E166" t="s">
-        <v>549</v>
+        <v>550</v>
       </c>
       <c r="F166" t="s">
         <v>13</v>
@@ -7092,9 +7097,9 @@
         <v>1</v>
       </c>
       <c r="H166" t="s">
-        <v>550</v>
-      </c>
-      <c r="I166" s="8">
+        <v>551</v>
+      </c>
+      <c r="I166" s="6">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update level1 logfile cf106601-ab4f-4af9-b045-5295fe67b37d
Signed-off-by: wangalexy <wangalexy@mailto.plus>
</commit_message>
<xml_diff>
--- a/results/GAIA/validation/gaia_validation.xlsx
+++ b/results/GAIA/validation/gaia_validation.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1037" uniqueCount="552">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1038" uniqueCount="552">
   <si>
     <t>Level</t>
   </si>
@@ -2799,7 +2799,7 @@
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="I51" sqref="I51"/>
+      <selection pane="bottomLeft" activeCell="J30" sqref="J30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10" defaultRowHeight="15.6"/>
@@ -4128,7 +4128,9 @@
       <c r="G51">
         <v>1</v>
       </c>
-      <c r="I51" s="6"/>
+      <c r="I51" s="6" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="52" ht="14.4" spans="1:9">
       <c r="A52" t="s">

</xml_diff>

<commit_message>
update level1 logfile c365c1c7-a3db-4d5e-a9a1-66f56eae7865
Signed-off-by: wangalexy <wangalexy@mailto.plus>
</commit_message>
<xml_diff>
--- a/results/GAIA/validation/gaia_validation.xlsx
+++ b/results/GAIA/validation/gaia_validation.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1038" uniqueCount="552">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1039" uniqueCount="552">
   <si>
     <t>Level</t>
   </si>
@@ -2799,7 +2799,7 @@
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="J30" sqref="J30"/>
+      <selection pane="bottomLeft" activeCell="J41" sqref="J41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10" defaultRowHeight="15.6"/>
@@ -3870,7 +3870,9 @@
       <c r="G41">
         <v>1</v>
       </c>
-      <c r="I41" s="6"/>
+      <c r="I41" s="6" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="42" ht="14.4" spans="1:9">
       <c r="A42" t="s">

</xml_diff>

<commit_message>
add level2 logfile db4fd70a-2d37-40ea-873f-9433dc5e301f
Signed-off-by: wangalexy <wangalexy@mailto.plus>
</commit_message>
<xml_diff>
--- a/results/GAIA/validation/gaia_validation.xlsx
+++ b/results/GAIA/validation/gaia_validation.xlsx
@@ -2799,7 +2799,7 @@
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="J41" sqref="J41"/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10" defaultRowHeight="15.6"/>
@@ -4305,7 +4305,7 @@
         <v>1</v>
       </c>
       <c r="I58">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="59" ht="14.4" customHeight="1" spans="1:9">

</xml_diff>

<commit_message>
add level2 logfile ecbc4f94-95a3-4cc7-b255-6741a458a625
Signed-off-by: wangalexy <wangalexy@mailto.plus>
</commit_message>
<xml_diff>
--- a/results/GAIA/validation/gaia_validation.xlsx
+++ b/results/GAIA/validation/gaia_validation.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1039" uniqueCount="552">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1040" uniqueCount="552">
   <si>
     <t>Level</t>
   </si>
@@ -5475,7 +5475,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" ht="14.4" customHeight="1" spans="1:7">
+    <row r="105" ht="14.4" customHeight="1" spans="1:9">
       <c r="A105" t="s">
         <v>176</v>
       </c>
@@ -5496,6 +5496,9 @@
       </c>
       <c r="G105">
         <v>1</v>
+      </c>
+      <c r="I105" s="2" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="106" ht="14.4" customHeight="1" spans="1:9">

</xml_diff>

<commit_message>
add level2 logfile 08cae58d-4084-4616-b6dd-dd6534e4825b
Signed-off-by: wangalexy <wangalexy@mailto.plus>
</commit_message>
<xml_diff>
--- a/results/GAIA/validation/gaia_validation.xlsx
+++ b/results/GAIA/validation/gaia_validation.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1040" uniqueCount="552">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1041" uniqueCount="552">
   <si>
     <t>Level</t>
   </si>
@@ -5380,7 +5380,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="101" ht="14.4" customHeight="1" spans="1:7">
+    <row r="101" ht="14.4" customHeight="1" spans="1:9">
       <c r="A101" t="s">
         <v>176</v>
       </c>
@@ -5401,6 +5401,9 @@
       </c>
       <c r="G101">
         <v>1</v>
+      </c>
+      <c r="I101" s="2" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="102" ht="14.4" customHeight="1" spans="1:9">

</xml_diff>